<commit_message>
Update testing file more case added and reading cell value usage example in readme added.
</commit_message>
<xml_diff>
--- a/test/Workbook1.xlsx
+++ b/test/Workbook1.xlsx
@@ -315,25 +315,6 @@
               </a:effectLst>
             </c:spPr>
           </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="20000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-            </c:spPr>
-          </c:dPt>
           <c:dLbls>
             <c:spPr>
               <a:pattFill prst="pct75">
@@ -408,22 +389,19 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$A$1:$A$5</c:f>
+              <c:f>Sheet2!$A$2:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Monitor</c:v>
+                  <c:v>&gt; 23 Inch</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>&gt; 23 Inch</c:v>
+                  <c:v>20-23 Inch</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20-23 Inch</c:v>
+                  <c:v>17-20 Inch</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17-20 Inch</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>&lt; 17 Inch</c:v>
                 </c:pt>
               </c:strCache>
@@ -431,20 +409,20 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$1:$B$5</c:f>
+              <c:f>Sheet2!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>19.0</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.0</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.0</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>21.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -713,40 +691,37 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$C$1:$C$11</c:f>
+              <c:f>Sheet2!$C$2:$C$11</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Brand</c:v>
+                  <c:v>HP</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>HP</c:v>
+                  <c:v>DELL</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>DELL</c:v>
+                  <c:v>Lenove</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Lenove</c:v>
+                  <c:v>SONY</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>SONY</c:v>
+                  <c:v>Acer</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Acer</c:v>
+                  <c:v>IBM</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>IBM</c:v>
+                  <c:v>ASUS</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>ASUS</c:v>
+                  <c:v>Apple</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Apple</c:v>
+                  <c:v>SAMSUNG</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>SAMSUNG</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>Other</c:v>
                 </c:pt>
               </c:strCache>
@@ -754,38 +729,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$D$1:$D$11</c:f>
+              <c:f>Sheet2!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>200.0</c:v>
+                </c:pt>
                 <c:pt idx="1">
+                  <c:v>450.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>200.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>450.0</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>200.0</c:v>
+                  <c:v>510.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>510.0</c:v>
+                  <c:v>315.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>315.0</c:v>
+                  <c:v>127.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>127.0</c:v>
+                  <c:v>89.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>89.0</c:v>
+                  <c:v>348.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>348.0</c:v>
+                  <c:v>53.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>53.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>37.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -803,11 +778,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="109775520"/>
-        <c:axId val="-307408000"/>
+        <c:axId val="-493998416"/>
+        <c:axId val="-493993888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="109775520"/>
+        <c:axId val="-493998416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -850,7 +825,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-307408000"/>
+        <c:crossAx val="-493993888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -858,7 +833,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-307408000"/>
+        <c:axId val="-493993888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -908,7 +883,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="109775520"/>
+        <c:crossAx val="-493998416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2598,8 +2573,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C11" s="4" t="s">
-        <v>15</v>
+      <c r="C11" s="4" t="str">
+        <v>Other</v>
       </c>
       <c r="D11" s="4">
         <v>37</v>

</xml_diff>

<commit_message>
Open file error return added and UpdateLinkedValue function added to fix linked values within a spreadsheet are not updating.
</commit_message>
<xml_diff>
--- a/test/Workbook1.xlsx
+++ b/test/Workbook1.xlsx
@@ -2450,7 +2450,17 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="19" spans="2:2">
+      <c r="A19" t="str">
+        <v>Total:</v>
+      </c>
+      <c r="B19">
+        <f>SUM(Sheet2!D2,Sheet2!D11)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix zoom scale and page layout view setting of XLSX.
</commit_message>
<xml_diff>
--- a/test/Workbook1.xlsx
+++ b/test/Workbook1.xlsx
@@ -1,29 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27417"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xuri/Sites/repo/excelize/test/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookPr date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="13220" yWindow="6260" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView activeTab="1" tabRatio="500" windowHeight="16880" windowWidth="28160" xWindow="13220" yWindow="6260"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="TestSheet" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="150000"/>
+  <fileRecoveryPr repairLoad="0"/>
 </workbook>
 </file>
 
@@ -2442,14 +2433,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr filterMode="false"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="false" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="16"/>
   <sheetData>
     <row r="19" spans="2:2">
       <c r="A19" t="str">
@@ -2457,36 +2449,983 @@
       </c>
       <c r="B19">
         <f>SUM(Sheet2!D2,Sheet2!D11)</f>
-        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="false" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="0" firstPageNumber="0" fitToWidth="0" fitToHeight="0" usePrinterDefaults="false" blackAndWhite="false" draft="false" useFirstPageNumber="false" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter differentFirst="false" differentOddEven="false"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr filterMode="false"/>
+  <dimension ref=""/>
+  <sheetViews/>
+  <sheetFormatPr defaultRowHeight="0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+      <c r="B1"/>
+    </row>
+    <row r="2">
+      <c r="A2"/>
+      <c r="B2"/>
+    </row>
+    <row r="3">
+      <c r="A3"/>
+      <c r="B3"/>
+    </row>
+    <row r="4">
+      <c r="A4"/>
+      <c r="B4"/>
+    </row>
+    <row r="5">
+      <c r="A5"/>
+      <c r="B5"/>
+    </row>
+    <row r="6">
+      <c r="A6"/>
+      <c r="B6"/>
+    </row>
+    <row r="7">
+      <c r="A7"/>
+      <c r="B7"/>
+    </row>
+    <row r="8">
+      <c r="A8"/>
+      <c r="B8"/>
+    </row>
+    <row r="9">
+      <c r="A9"/>
+      <c r="B9"/>
+    </row>
+    <row r="10">
+      <c r="A10"/>
+      <c r="B10"/>
+    </row>
+    <row r="11">
+      <c r="A11"/>
+      <c r="B11"/>
+    </row>
+    <row r="12">
+      <c r="A12"/>
+      <c r="B12"/>
+    </row>
+    <row r="13">
+      <c r="A13"/>
+      <c r="B13"/>
+    </row>
+    <row r="14">
+      <c r="A14"/>
+      <c r="B14"/>
+    </row>
+    <row r="15">
+      <c r="A15"/>
+      <c r="B15"/>
+    </row>
+    <row r="16">
+      <c r="A16"/>
+      <c r="B16"/>
+    </row>
+    <row r="17">
+      <c r="A17"/>
+      <c r="B17"/>
+    </row>
+    <row r="18">
+      <c r="A18"/>
+      <c r="B18"/>
+    </row>
+    <row r="19">
+      <c r="A19"/>
+      <c r="B19"/>
+    </row>
+    <row r="20">
+      <c r="A20"/>
+      <c r="B20"/>
+    </row>
+    <row r="21">
+      <c r="A21"/>
+      <c r="B21"/>
+    </row>
+    <row r="22">
+      <c r="A22"/>
+      <c r="B22"/>
+    </row>
+    <row r="23">
+      <c r="A23"/>
+      <c r="B23"/>
+    </row>
+    <row r="24">
+      <c r="A24"/>
+      <c r="B24"/>
+    </row>
+    <row r="25">
+      <c r="A25"/>
+      <c r="B25"/>
+    </row>
+    <row r="26">
+      <c r="A26"/>
+      <c r="B26"/>
+    </row>
+    <row r="27">
+      <c r="A27"/>
+      <c r="B27"/>
+    </row>
+    <row r="28">
+      <c r="A28"/>
+      <c r="B28"/>
+    </row>
+    <row r="29">
+      <c r="A29"/>
+      <c r="B29"/>
+    </row>
+    <row r="30">
+      <c r="A30"/>
+      <c r="B30"/>
+    </row>
+    <row r="31">
+      <c r="A31"/>
+      <c r="B31"/>
+    </row>
+    <row r="32">
+      <c r="A32"/>
+      <c r="B32"/>
+    </row>
+    <row r="33">
+      <c r="A33"/>
+      <c r="B33"/>
+    </row>
+    <row r="34">
+      <c r="A34"/>
+      <c r="B34"/>
+    </row>
+    <row r="35">
+      <c r="A35"/>
+      <c r="B35"/>
+    </row>
+    <row r="36">
+      <c r="A36"/>
+      <c r="B36"/>
+    </row>
+    <row r="37">
+      <c r="A37"/>
+      <c r="B37"/>
+    </row>
+    <row r="38">
+      <c r="A38"/>
+      <c r="B38"/>
+    </row>
+    <row r="39">
+      <c r="A39"/>
+      <c r="B39"/>
+    </row>
+    <row r="40">
+      <c r="A40"/>
+      <c r="B40"/>
+    </row>
+    <row r="41">
+      <c r="A41"/>
+      <c r="B41"/>
+    </row>
+    <row r="42">
+      <c r="A42"/>
+      <c r="B42"/>
+    </row>
+    <row r="43">
+      <c r="A43"/>
+      <c r="B43"/>
+    </row>
+    <row r="44">
+      <c r="A44"/>
+      <c r="B44"/>
+    </row>
+    <row r="45">
+      <c r="A45"/>
+      <c r="B45"/>
+    </row>
+    <row r="46">
+      <c r="A46"/>
+      <c r="B46"/>
+    </row>
+    <row r="47">
+      <c r="A47"/>
+      <c r="B47"/>
+    </row>
+    <row r="48">
+      <c r="A48"/>
+      <c r="B48"/>
+    </row>
+    <row r="49">
+      <c r="A49"/>
+      <c r="B49"/>
+    </row>
+    <row r="50">
+      <c r="A50"/>
+      <c r="B50"/>
+    </row>
+    <row r="51">
+      <c r="A51"/>
+      <c r="B51"/>
+    </row>
+    <row r="52">
+      <c r="A52"/>
+      <c r="B52"/>
+    </row>
+    <row r="53">
+      <c r="A53"/>
+      <c r="B53"/>
+    </row>
+    <row r="54">
+      <c r="A54"/>
+      <c r="B54"/>
+    </row>
+    <row r="55">
+      <c r="A55"/>
+      <c r="B55"/>
+    </row>
+    <row r="56">
+      <c r="A56"/>
+      <c r="B56"/>
+    </row>
+    <row r="57">
+      <c r="A57"/>
+      <c r="B57"/>
+    </row>
+    <row r="58">
+      <c r="A58"/>
+      <c r="B58"/>
+    </row>
+    <row r="59">
+      <c r="A59"/>
+      <c r="B59"/>
+    </row>
+    <row r="60">
+      <c r="A60"/>
+      <c r="B60"/>
+    </row>
+    <row r="61">
+      <c r="A61"/>
+      <c r="B61"/>
+    </row>
+    <row r="62">
+      <c r="A62"/>
+      <c r="B62"/>
+    </row>
+    <row r="63">
+      <c r="A63"/>
+      <c r="B63"/>
+    </row>
+    <row r="64">
+      <c r="A64"/>
+      <c r="B64"/>
+    </row>
+    <row r="65">
+      <c r="A65"/>
+      <c r="B65"/>
+    </row>
+    <row r="66">
+      <c r="A66"/>
+      <c r="B66"/>
+    </row>
+    <row r="67">
+      <c r="A67"/>
+      <c r="B67"/>
+    </row>
+    <row r="68">
+      <c r="A68"/>
+      <c r="B68"/>
+    </row>
+    <row r="69">
+      <c r="A69"/>
+      <c r="B69"/>
+    </row>
+    <row r="70">
+      <c r="A70"/>
+      <c r="B70"/>
+    </row>
+    <row r="71">
+      <c r="A71"/>
+      <c r="B71"/>
+    </row>
+    <row r="72">
+      <c r="A72"/>
+      <c r="B72"/>
+    </row>
+    <row r="73">
+      <c r="A73"/>
+      <c r="B73"/>
+    </row>
+    <row r="74">
+      <c r="A74"/>
+      <c r="B74"/>
+    </row>
+    <row r="75">
+      <c r="A75"/>
+      <c r="B75"/>
+    </row>
+    <row r="76">
+      <c r="A76"/>
+      <c r="B76"/>
+    </row>
+    <row r="77">
+      <c r="A77"/>
+      <c r="B77"/>
+    </row>
+    <row r="78">
+      <c r="A78"/>
+      <c r="B78"/>
+    </row>
+    <row r="79">
+      <c r="A79"/>
+      <c r="B79"/>
+    </row>
+    <row r="80">
+      <c r="A80"/>
+      <c r="B80"/>
+    </row>
+    <row r="81">
+      <c r="A81"/>
+      <c r="B81"/>
+    </row>
+    <row r="82">
+      <c r="A82"/>
+      <c r="B82"/>
+    </row>
+    <row r="83">
+      <c r="A83"/>
+      <c r="B83"/>
+    </row>
+    <row r="84">
+      <c r="A84"/>
+      <c r="B84"/>
+    </row>
+    <row r="85">
+      <c r="A85"/>
+      <c r="B85"/>
+    </row>
+    <row r="86">
+      <c r="A86"/>
+      <c r="B86"/>
+    </row>
+    <row r="87">
+      <c r="A87"/>
+      <c r="B87"/>
+    </row>
+    <row r="88">
+      <c r="A88"/>
+      <c r="B88"/>
+    </row>
+    <row r="89">
+      <c r="A89"/>
+      <c r="B89"/>
+    </row>
+    <row r="90">
+      <c r="A90"/>
+      <c r="B90"/>
+    </row>
+    <row r="91">
+      <c r="A91"/>
+      <c r="B91"/>
+    </row>
+    <row r="92">
+      <c r="A92"/>
+      <c r="B92"/>
+    </row>
+    <row r="93">
+      <c r="A93"/>
+      <c r="B93"/>
+    </row>
+    <row r="94">
+      <c r="A94"/>
+      <c r="B94"/>
+    </row>
+    <row r="95">
+      <c r="A95"/>
+      <c r="B95"/>
+    </row>
+    <row r="96">
+      <c r="A96"/>
+      <c r="B96"/>
+    </row>
+    <row r="97">
+      <c r="A97"/>
+      <c r="B97"/>
+    </row>
+    <row r="98">
+      <c r="A98"/>
+      <c r="B98"/>
+    </row>
+    <row r="99">
+      <c r="A99"/>
+      <c r="B99"/>
+    </row>
+    <row r="100">
+      <c r="A100"/>
+      <c r="B100"/>
+    </row>
+    <row r="101">
+      <c r="A101"/>
+      <c r="B101"/>
+    </row>
+    <row r="102">
+      <c r="A102"/>
+      <c r="B102"/>
+    </row>
+    <row r="103">
+      <c r="A103"/>
+      <c r="B103"/>
+    </row>
+    <row r="104">
+      <c r="A104"/>
+      <c r="B104"/>
+    </row>
+    <row r="105">
+      <c r="A105"/>
+      <c r="B105"/>
+    </row>
+    <row r="106">
+      <c r="A106"/>
+      <c r="B106"/>
+    </row>
+    <row r="107">
+      <c r="A107"/>
+      <c r="B107"/>
+    </row>
+    <row r="108">
+      <c r="A108"/>
+      <c r="B108"/>
+    </row>
+    <row r="109">
+      <c r="A109"/>
+      <c r="B109"/>
+    </row>
+    <row r="110">
+      <c r="A110"/>
+      <c r="B110"/>
+    </row>
+    <row r="111">
+      <c r="A111"/>
+      <c r="B111"/>
+    </row>
+    <row r="112">
+      <c r="A112"/>
+      <c r="B112"/>
+    </row>
+    <row r="113">
+      <c r="A113"/>
+      <c r="B113"/>
+    </row>
+    <row r="114">
+      <c r="A114"/>
+      <c r="B114"/>
+    </row>
+    <row r="115">
+      <c r="A115"/>
+      <c r="B115"/>
+    </row>
+    <row r="116">
+      <c r="A116"/>
+      <c r="B116"/>
+    </row>
+    <row r="117">
+      <c r="A117"/>
+      <c r="B117"/>
+    </row>
+    <row r="118">
+      <c r="A118"/>
+      <c r="B118"/>
+    </row>
+    <row r="119">
+      <c r="A119"/>
+      <c r="B119"/>
+    </row>
+    <row r="120">
+      <c r="A120"/>
+      <c r="B120"/>
+    </row>
+    <row r="121">
+      <c r="A121"/>
+      <c r="B121"/>
+    </row>
+    <row r="122">
+      <c r="A122"/>
+      <c r="B122"/>
+    </row>
+    <row r="123">
+      <c r="A123"/>
+      <c r="B123"/>
+    </row>
+    <row r="124">
+      <c r="A124"/>
+      <c r="B124"/>
+    </row>
+    <row r="125">
+      <c r="A125"/>
+      <c r="B125"/>
+    </row>
+    <row r="126">
+      <c r="A126"/>
+      <c r="B126"/>
+    </row>
+    <row r="127">
+      <c r="A127"/>
+      <c r="B127"/>
+    </row>
+    <row r="128">
+      <c r="A128"/>
+      <c r="B128"/>
+    </row>
+    <row r="129">
+      <c r="A129"/>
+      <c r="B129"/>
+    </row>
+    <row r="130">
+      <c r="A130"/>
+      <c r="B130"/>
+    </row>
+    <row r="131">
+      <c r="A131"/>
+      <c r="B131"/>
+    </row>
+    <row r="132">
+      <c r="A132"/>
+      <c r="B132"/>
+    </row>
+    <row r="133">
+      <c r="A133"/>
+      <c r="B133"/>
+    </row>
+    <row r="134">
+      <c r="A134"/>
+      <c r="B134"/>
+    </row>
+    <row r="135">
+      <c r="A135"/>
+      <c r="B135"/>
+    </row>
+    <row r="136">
+      <c r="A136"/>
+      <c r="B136"/>
+    </row>
+    <row r="137">
+      <c r="A137"/>
+      <c r="B137"/>
+    </row>
+    <row r="138">
+      <c r="A138"/>
+      <c r="B138"/>
+    </row>
+    <row r="139">
+      <c r="A139"/>
+      <c r="B139"/>
+    </row>
+    <row r="140">
+      <c r="A140"/>
+      <c r="B140"/>
+    </row>
+    <row r="141">
+      <c r="A141"/>
+      <c r="B141"/>
+    </row>
+    <row r="142">
+      <c r="A142"/>
+      <c r="B142"/>
+    </row>
+    <row r="143">
+      <c r="A143"/>
+      <c r="B143"/>
+    </row>
+    <row r="144">
+      <c r="A144"/>
+      <c r="B144"/>
+    </row>
+    <row r="145">
+      <c r="A145"/>
+      <c r="B145"/>
+    </row>
+    <row r="146">
+      <c r="A146"/>
+      <c r="B146"/>
+    </row>
+    <row r="147">
+      <c r="A147"/>
+      <c r="B147"/>
+    </row>
+    <row r="148">
+      <c r="A148"/>
+      <c r="B148"/>
+    </row>
+    <row r="149">
+      <c r="A149"/>
+      <c r="B149"/>
+    </row>
+    <row r="150">
+      <c r="A150"/>
+      <c r="B150"/>
+    </row>
+    <row r="151">
+      <c r="A151"/>
+      <c r="B151"/>
+    </row>
+    <row r="152">
+      <c r="A152"/>
+      <c r="B152"/>
+    </row>
+    <row r="153">
+      <c r="A153"/>
+      <c r="B153"/>
+    </row>
+    <row r="154">
+      <c r="A154"/>
+      <c r="B154"/>
+    </row>
+    <row r="155">
+      <c r="A155"/>
+      <c r="B155"/>
+    </row>
+    <row r="156">
+      <c r="A156"/>
+      <c r="B156"/>
+    </row>
+    <row r="157">
+      <c r="A157"/>
+      <c r="B157"/>
+    </row>
+    <row r="158">
+      <c r="A158"/>
+      <c r="B158"/>
+    </row>
+    <row r="159">
+      <c r="A159"/>
+      <c r="B159"/>
+    </row>
+    <row r="160">
+      <c r="A160"/>
+      <c r="B160"/>
+    </row>
+    <row r="161">
+      <c r="A161"/>
+      <c r="B161"/>
+    </row>
+    <row r="162">
+      <c r="A162"/>
+      <c r="B162"/>
+    </row>
+    <row r="163">
+      <c r="A163"/>
+      <c r="B163"/>
+    </row>
+    <row r="164">
+      <c r="A164"/>
+      <c r="B164"/>
+    </row>
+    <row r="165">
+      <c r="A165"/>
+      <c r="B165"/>
+    </row>
+    <row r="166">
+      <c r="A166"/>
+      <c r="B166"/>
+    </row>
+    <row r="167">
+      <c r="A167"/>
+      <c r="B167"/>
+    </row>
+    <row r="168">
+      <c r="A168"/>
+      <c r="B168"/>
+    </row>
+    <row r="169">
+      <c r="A169"/>
+      <c r="B169"/>
+    </row>
+    <row r="170">
+      <c r="A170"/>
+      <c r="B170"/>
+    </row>
+    <row r="171">
+      <c r="A171"/>
+      <c r="B171"/>
+    </row>
+    <row r="172">
+      <c r="A172"/>
+      <c r="B172"/>
+    </row>
+    <row r="173">
+      <c r="A173"/>
+      <c r="B173"/>
+    </row>
+    <row r="174">
+      <c r="A174"/>
+      <c r="B174"/>
+    </row>
+    <row r="175">
+      <c r="A175"/>
+      <c r="B175"/>
+    </row>
+    <row r="176">
+      <c r="A176"/>
+      <c r="B176"/>
+    </row>
+    <row r="177">
+      <c r="A177"/>
+      <c r="B177"/>
+    </row>
+    <row r="178">
+      <c r="A178"/>
+      <c r="B178"/>
+    </row>
+    <row r="179">
+      <c r="A179"/>
+      <c r="B179"/>
+    </row>
+    <row r="180">
+      <c r="A180"/>
+      <c r="B180"/>
+    </row>
+    <row r="181">
+      <c r="A181"/>
+      <c r="B181"/>
+    </row>
+    <row r="182">
+      <c r="A182"/>
+      <c r="B182"/>
+    </row>
+    <row r="183">
+      <c r="A183"/>
+      <c r="B183"/>
+    </row>
+    <row r="184">
+      <c r="A184"/>
+      <c r="B184"/>
+    </row>
+    <row r="185">
+      <c r="A185"/>
+      <c r="B185"/>
+    </row>
+    <row r="186">
+      <c r="A186"/>
+      <c r="B186"/>
+    </row>
+    <row r="187">
+      <c r="A187"/>
+      <c r="B187"/>
+    </row>
+    <row r="188">
+      <c r="A188"/>
+      <c r="B188"/>
+    </row>
+    <row r="189">
+      <c r="A189"/>
+      <c r="B189"/>
+    </row>
+    <row r="190">
+      <c r="A190"/>
+      <c r="B190"/>
+    </row>
+    <row r="191">
+      <c r="A191"/>
+      <c r="B191"/>
+    </row>
+    <row r="192">
+      <c r="A192"/>
+      <c r="B192"/>
+    </row>
+    <row r="193">
+      <c r="A193"/>
+      <c r="B193"/>
+    </row>
+    <row r="194">
+      <c r="A194"/>
+      <c r="B194"/>
+    </row>
+    <row r="195">
+      <c r="A195"/>
+      <c r="B195"/>
+    </row>
+    <row r="196">
+      <c r="A196"/>
+      <c r="B196"/>
+    </row>
+    <row r="197">
+      <c r="A197"/>
+      <c r="B197"/>
+    </row>
+    <row r="198">
+      <c r="A198"/>
+      <c r="B198"/>
+    </row>
+    <row r="199">
+      <c r="A199"/>
+      <c r="B199"/>
+    </row>
+    <row r="200">
+      <c r="A200"/>
+      <c r="B200"/>
+    </row>
+    <row r="201">
+      <c r="A201"/>
+      <c r="B201"/>
+    </row>
+    <row r="202">
+      <c r="A202"/>
+      <c r="B202"/>
+    </row>
+    <row r="203">
+      <c r="A203"/>
+      <c r="B203"/>
+    </row>
+    <row r="204">
+      <c r="A204"/>
+      <c r="B204"/>
+    </row>
+    <row r="205">
+      <c r="A205"/>
+      <c r="B205"/>
+    </row>
+    <row r="206">
+      <c r="A206"/>
+      <c r="B206"/>
+    </row>
+    <row r="207">
+      <c r="A207"/>
+      <c r="B207"/>
+    </row>
+    <row r="208">
+      <c r="A208"/>
+      <c r="B208"/>
+    </row>
+    <row r="209">
+      <c r="A209"/>
+      <c r="B209"/>
+    </row>
+    <row r="210">
+      <c r="A210"/>
+      <c r="B210"/>
+    </row>
+    <row r="211">
+      <c r="A211"/>
+      <c r="B211"/>
+    </row>
+    <row r="212">
+      <c r="A212"/>
+      <c r="B212"/>
+    </row>
+    <row r="213">
+      <c r="A213"/>
+      <c r="B213"/>
+    </row>
+    <row r="214">
+      <c r="A214"/>
+      <c r="B214"/>
+    </row>
+    <row r="215">
+      <c r="A215"/>
+      <c r="B215"/>
+    </row>
+    <row r="216">
+      <c r="A216"/>
+      <c r="B216"/>
+    </row>
+    <row r="217">
+      <c r="A217"/>
+      <c r="B217"/>
+    </row>
+    <row r="218">
+      <c r="A218"/>
+      <c r="B218"/>
+    </row>
+    <row r="219">
+      <c r="A219"/>
+      <c r="B219"/>
+    </row>
+    <row r="220">
+      <c r="A220"/>
+      <c r="B220"/>
+    </row>
+    <row r="221">
+      <c r="A221"/>
+      <c r="B221"/>
+    </row>
+    <row r="222">
+      <c r="A222"/>
+      <c r="B222"/>
+    </row>
+    <row r="223">
+      <c r="A223"/>
+      <c r="B223"/>
+    </row>
+    <row r="224">
+      <c r="A224"/>
+      <c r="B224"/>
+    </row>
+    <row r="225">
+      <c r="A225"/>
+      <c r="B225"/>
+    </row>
+    <row r="226">
+      <c r="A226"/>
+      <c r="B226"/>
+    </row>
+    <row r="227">
+      <c r="A227"/>
+      <c r="B227"/>
+    </row>
+    <row r="228">
+      <c r="A228"/>
+      <c r="B228"/>
+    </row>
+    <row r="229">
+      <c r="A229"/>
+      <c r="B229"/>
+    </row>
+    <row r="230">
+      <c r="A230"/>
+      <c r="B230" t="str">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup scale="0" firstPageNumber="0" fitToWidth="0" fitToHeight="0" usePrinterDefaults="false" blackAndWhite="false" draft="false" useFirstPageNumber="false" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter differentFirst="false" differentOddEven="false"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr filterMode="false"/>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
+    <row r="1" spans="1:4" ht="17">
+      <c r="A1" s="1">
+        <v>100</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E1"/>
+      <c r="F1" t="str">
+        <v>Hello</v>
+      </c>
+      <c r="G1" t="str">
+        <v>World</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -2499,8 +3438,13 @@
       <c r="D2" s="4">
         <v>200</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E2"/>
+      <c r="F2">
+        <v>42</v>
+      </c>
+      <c r="G2" t="str"/>
+    </row>
+    <row r="3" spans="1:4" ht="17">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2513,8 +3457,11 @@
       <c r="D3" s="4">
         <v>450</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+    </row>
+    <row r="4" spans="1:4" ht="17">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -2527,8 +3474,11 @@
       <c r="D4" s="4">
         <v>200</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+    </row>
+    <row r="5" spans="1:4" ht="17">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -2541,57 +3491,2222 @@
       <c r="D5" s="4">
         <v>510</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6"/>
+      <c r="B6"/>
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="4">
         <v>315</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7"/>
+      <c r="B7"/>
       <c r="C7" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="4">
         <v>127</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8"/>
+      <c r="B8"/>
       <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="4">
         <v>89</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9"/>
+      <c r="B9"/>
       <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="4">
         <v>348</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10"/>
+      <c r="B10"/>
       <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="4">
         <v>53</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11"/>
+      <c r="B11"/>
       <c r="C11" s="4" t="str">
-        <v>Other</v>
+        <v>Knowns</v>
       </c>
       <c r="D11" s="4">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+    </row>
   </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="false" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="0" firstPageNumber="0" fitToWidth="0" fitToHeight="0" usePrinterDefaults="false" blackAndWhite="false" draft="false" useFirstPageNumber="false" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter differentFirst="false" differentOddEven="false"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr filterMode="false"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="false" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+      <c r="B1"/>
+      <c r="C1" t="str">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2" t="str">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="C3" t="str">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4" t="str">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6" t="str">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7" t="str">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8" t="str">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9" t="str">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10" t="str">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11" t="str">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12" t="str">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13" t="str">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14" t="str">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15" t="str">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16" t="str">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17" t="str">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18" t="str">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19" t="str">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20" t="str">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21" t="str">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22" t="str">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>10</v>
+      </c>
+      <c r="B23"/>
+      <c r="C23" t="str">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24" t="str">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25" t="str">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26" t="str">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27" t="str">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28" t="str">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29" t="str">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30"/>
+      <c r="B30"/>
+      <c r="C30" t="str">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31" t="str">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32"/>
+      <c r="B32"/>
+      <c r="C32" t="str">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33"/>
+      <c r="B33"/>
+      <c r="C33" t="str">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34" t="str">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35"/>
+      <c r="B35"/>
+      <c r="C35" t="str">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36"/>
+      <c r="B36"/>
+      <c r="C36" t="str">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37"/>
+      <c r="B37"/>
+      <c r="C37" t="str">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38"/>
+      <c r="B38"/>
+      <c r="C38" t="str">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39"/>
+      <c r="B39"/>
+      <c r="C39" t="str">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40"/>
+      <c r="B40"/>
+      <c r="C40" t="str">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41"/>
+      <c r="B41"/>
+      <c r="C41" t="str">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42"/>
+      <c r="B42"/>
+      <c r="C42" t="str">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43"/>
+      <c r="B43"/>
+      <c r="C43" t="str">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44"/>
+      <c r="B44"/>
+      <c r="C44" t="str">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45"/>
+      <c r="B45"/>
+      <c r="C45" t="str">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46"/>
+      <c r="B46"/>
+      <c r="C46" t="str">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47"/>
+      <c r="B47"/>
+      <c r="C47" t="str">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48"/>
+      <c r="B48"/>
+      <c r="C48" t="str">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49"/>
+      <c r="B49"/>
+      <c r="C49" t="str">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50"/>
+      <c r="B50"/>
+      <c r="C50" t="str">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51"/>
+      <c r="B51"/>
+      <c r="C51" t="str">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52"/>
+      <c r="B52"/>
+      <c r="C52" t="str">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53"/>
+      <c r="B53"/>
+      <c r="C53" t="str">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54"/>
+      <c r="B54"/>
+      <c r="C54" t="str">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55"/>
+      <c r="B55"/>
+      <c r="C55" t="str">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56"/>
+      <c r="B56"/>
+      <c r="C56" t="str">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57"/>
+      <c r="B57"/>
+      <c r="C57" t="str">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58"/>
+      <c r="B58"/>
+      <c r="C58" t="str">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59"/>
+      <c r="B59"/>
+      <c r="C59" t="str">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60"/>
+      <c r="B60"/>
+      <c r="C60" t="str">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61"/>
+      <c r="B61"/>
+      <c r="C61" t="str">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62"/>
+      <c r="B62"/>
+      <c r="C62" t="str">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63"/>
+      <c r="B63"/>
+      <c r="C63" t="str">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64"/>
+      <c r="B64"/>
+      <c r="C64" t="str">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65"/>
+      <c r="B65"/>
+      <c r="C65" t="str">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66"/>
+      <c r="B66"/>
+      <c r="C66" t="str">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67"/>
+      <c r="B67"/>
+      <c r="C67" t="str">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68"/>
+      <c r="B68"/>
+      <c r="C68" t="str">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69"/>
+      <c r="B69"/>
+      <c r="C69" t="str">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70"/>
+      <c r="B70"/>
+      <c r="C70" t="str">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71"/>
+      <c r="B71"/>
+      <c r="C71" t="str">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72"/>
+      <c r="B72"/>
+      <c r="C72" t="str">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73"/>
+      <c r="B73"/>
+      <c r="C73" t="str">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74"/>
+      <c r="B74"/>
+      <c r="C74" t="str">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75"/>
+      <c r="B75"/>
+      <c r="C75" t="str">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76"/>
+      <c r="B76"/>
+      <c r="C76" t="str">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77"/>
+      <c r="B77"/>
+      <c r="C77" t="str">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78"/>
+      <c r="B78"/>
+      <c r="C78" t="str">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79"/>
+      <c r="B79"/>
+      <c r="C79" t="str">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80"/>
+      <c r="B80"/>
+      <c r="C80" t="str">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81"/>
+      <c r="B81"/>
+      <c r="C81" t="str">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82"/>
+      <c r="B82"/>
+      <c r="C82" t="str">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83"/>
+      <c r="B83"/>
+      <c r="C83" t="str">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84"/>
+      <c r="B84"/>
+      <c r="C84" t="str">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85"/>
+      <c r="B85"/>
+      <c r="C85" t="str">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86"/>
+      <c r="B86"/>
+      <c r="C86" t="str">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87"/>
+      <c r="B87"/>
+      <c r="C87" t="str">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88"/>
+      <c r="B88"/>
+      <c r="C88" t="str">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89"/>
+      <c r="B89"/>
+      <c r="C89" t="str">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90"/>
+      <c r="B90"/>
+      <c r="C90" t="str">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91"/>
+      <c r="B91"/>
+      <c r="C91" t="str">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92"/>
+      <c r="B92"/>
+      <c r="C92" t="str">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93"/>
+      <c r="B93"/>
+      <c r="C93" t="str">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94"/>
+      <c r="B94"/>
+      <c r="C94" t="str">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95"/>
+      <c r="B95"/>
+      <c r="C95" t="str">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96"/>
+      <c r="B96"/>
+      <c r="C96" t="str">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97"/>
+      <c r="B97"/>
+      <c r="C97" t="str">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98"/>
+      <c r="B98"/>
+      <c r="C98" t="str">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99"/>
+      <c r="B99"/>
+      <c r="C99" t="str">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100"/>
+      <c r="B100"/>
+      <c r="C100" t="str">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101"/>
+      <c r="B101"/>
+      <c r="C101" t="str">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102"/>
+      <c r="B102"/>
+      <c r="C102" t="str">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103"/>
+      <c r="B103"/>
+      <c r="C103" t="str">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104"/>
+      <c r="B104"/>
+      <c r="C104" t="str">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105"/>
+      <c r="B105"/>
+      <c r="C105" t="str">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106"/>
+      <c r="B106"/>
+      <c r="C106" t="str">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107"/>
+      <c r="B107"/>
+      <c r="C107" t="str">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108"/>
+      <c r="B108"/>
+      <c r="C108" t="str">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109"/>
+      <c r="B109"/>
+      <c r="C109" t="str">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110"/>
+      <c r="B110"/>
+      <c r="C110" t="str">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111"/>
+      <c r="B111"/>
+      <c r="C111" t="str">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112"/>
+      <c r="B112"/>
+      <c r="C112" t="str">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113"/>
+      <c r="B113"/>
+      <c r="C113" t="str">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114"/>
+      <c r="B114"/>
+      <c r="C114" t="str">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115"/>
+      <c r="B115"/>
+      <c r="C115" t="str">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116"/>
+      <c r="B116"/>
+      <c r="C116" t="str">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117"/>
+      <c r="B117"/>
+      <c r="C117" t="str">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118"/>
+      <c r="B118"/>
+      <c r="C118" t="str">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119"/>
+      <c r="B119"/>
+      <c r="C119" t="str">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120"/>
+      <c r="B120"/>
+      <c r="C120" t="str">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121"/>
+      <c r="B121"/>
+      <c r="C121" t="str">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122"/>
+      <c r="B122"/>
+      <c r="C122" t="str">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123"/>
+      <c r="B123"/>
+      <c r="C123" t="str">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124"/>
+      <c r="B124"/>
+      <c r="C124" t="str">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125"/>
+      <c r="B125"/>
+      <c r="C125" t="str">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126"/>
+      <c r="B126"/>
+      <c r="C126" t="str">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127"/>
+      <c r="B127"/>
+      <c r="C127" t="str">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128"/>
+      <c r="B128"/>
+      <c r="C128" t="str">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129"/>
+      <c r="B129"/>
+      <c r="C129" t="str">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130"/>
+      <c r="B130"/>
+      <c r="C130" t="str">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131"/>
+      <c r="B131"/>
+      <c r="C131" t="str">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132"/>
+      <c r="B132"/>
+      <c r="C132" t="str">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133"/>
+      <c r="B133"/>
+      <c r="C133" t="str">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134"/>
+      <c r="B134"/>
+      <c r="C134" t="str">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135"/>
+      <c r="B135"/>
+      <c r="C135" t="str">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136"/>
+      <c r="B136"/>
+      <c r="C136" t="str">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137"/>
+      <c r="B137"/>
+      <c r="C137" t="str">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138"/>
+      <c r="B138"/>
+      <c r="C138" t="str">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139"/>
+      <c r="B139"/>
+      <c r="C139" t="str">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140"/>
+      <c r="B140"/>
+      <c r="C140" t="str">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141"/>
+      <c r="B141"/>
+      <c r="C141" t="str">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142"/>
+      <c r="B142"/>
+      <c r="C142" t="str">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143"/>
+      <c r="B143"/>
+      <c r="C143" t="str">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144"/>
+      <c r="B144"/>
+      <c r="C144" t="str">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145"/>
+      <c r="B145"/>
+      <c r="C145" t="str">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146"/>
+      <c r="B146"/>
+      <c r="C146" t="str">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147"/>
+      <c r="B147"/>
+      <c r="C147" t="str">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148"/>
+      <c r="B148"/>
+      <c r="C148" t="str">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149"/>
+      <c r="B149"/>
+      <c r="C149" t="str">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150"/>
+      <c r="B150"/>
+      <c r="C150" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151"/>
+      <c r="B151"/>
+      <c r="C151" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152"/>
+      <c r="B152"/>
+      <c r="C152" t="str">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153"/>
+      <c r="B153"/>
+      <c r="C153" t="str">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154"/>
+      <c r="B154"/>
+      <c r="C154" t="str">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155"/>
+      <c r="B155"/>
+      <c r="C155" t="str">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156"/>
+      <c r="B156"/>
+      <c r="C156" t="str">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157"/>
+      <c r="B157"/>
+      <c r="C157" t="str">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158"/>
+      <c r="B158"/>
+      <c r="C158" t="str">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159"/>
+      <c r="B159"/>
+      <c r="C159" t="str">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160"/>
+      <c r="B160"/>
+      <c r="C160" t="str">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161"/>
+      <c r="B161"/>
+      <c r="C161" t="str">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162"/>
+      <c r="B162"/>
+      <c r="C162" t="str">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163"/>
+      <c r="B163"/>
+      <c r="C163" t="str">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164"/>
+      <c r="B164"/>
+      <c r="C164" t="str">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165"/>
+      <c r="B165"/>
+      <c r="C165" t="str">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166"/>
+      <c r="B166"/>
+      <c r="C166" t="str">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167"/>
+      <c r="B167"/>
+      <c r="C167" t="str">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168"/>
+      <c r="B168"/>
+      <c r="C168" t="str">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169"/>
+      <c r="B169"/>
+      <c r="C169" t="str">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170"/>
+      <c r="B170"/>
+      <c r="C170" t="str">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171"/>
+      <c r="B171"/>
+      <c r="C171" t="str">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172"/>
+      <c r="B172"/>
+      <c r="C172" t="str">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173"/>
+      <c r="B173"/>
+      <c r="C173" t="str">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174"/>
+      <c r="B174"/>
+      <c r="C174" t="str">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175"/>
+      <c r="B175"/>
+      <c r="C175" t="str">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176"/>
+      <c r="B176"/>
+      <c r="C176" t="str">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177"/>
+      <c r="B177"/>
+      <c r="C177" t="str">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178"/>
+      <c r="B178"/>
+      <c r="C178" t="str">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179"/>
+      <c r="B179"/>
+      <c r="C179" t="str">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180"/>
+      <c r="B180"/>
+      <c r="C180" t="str">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181"/>
+      <c r="B181"/>
+      <c r="C181" t="str">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182"/>
+      <c r="B182"/>
+      <c r="C182" t="str">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183"/>
+      <c r="B183"/>
+      <c r="C183" t="str">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184"/>
+      <c r="B184"/>
+      <c r="C184" t="str">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185"/>
+      <c r="B185"/>
+      <c r="C185" t="str">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186"/>
+      <c r="B186"/>
+      <c r="C186" t="str">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187"/>
+      <c r="B187"/>
+      <c r="C187" t="str">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188"/>
+      <c r="B188"/>
+      <c r="C188" t="str">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189"/>
+      <c r="B189"/>
+      <c r="C189" t="str">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190"/>
+      <c r="B190"/>
+      <c r="C190" t="str">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191"/>
+      <c r="B191"/>
+      <c r="C191" t="str">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192"/>
+      <c r="B192"/>
+      <c r="C192" t="str">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193"/>
+      <c r="B193"/>
+      <c r="C193" t="str">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194"/>
+      <c r="B194"/>
+      <c r="C194" t="str">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195"/>
+      <c r="B195"/>
+      <c r="C195" t="str">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196"/>
+      <c r="B196"/>
+      <c r="C196" t="str">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197"/>
+      <c r="B197"/>
+      <c r="C197" t="str">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198"/>
+      <c r="B198"/>
+      <c r="C198" t="str">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199"/>
+      <c r="B199"/>
+      <c r="C199" t="str">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200"/>
+      <c r="B200"/>
+      <c r="C200" t="str">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201"/>
+      <c r="B201"/>
+      <c r="C201" t="str">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202"/>
+      <c r="B202"/>
+      <c r="C202" t="str">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203"/>
+      <c r="B203"/>
+      <c r="C203" t="str">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204"/>
+      <c r="B204"/>
+      <c r="C204" t="str">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205"/>
+      <c r="B205"/>
+      <c r="C205" t="str">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206"/>
+      <c r="B206"/>
+      <c r="C206" t="str">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207"/>
+      <c r="B207"/>
+      <c r="C207" t="str">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208"/>
+      <c r="B208"/>
+      <c r="C208" t="str">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209"/>
+      <c r="B209"/>
+      <c r="C209" t="str">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210"/>
+      <c r="B210"/>
+      <c r="C210" t="str">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211"/>
+      <c r="B211"/>
+      <c r="C211" t="str">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212"/>
+      <c r="B212"/>
+      <c r="C212" t="str">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213"/>
+      <c r="B213"/>
+      <c r="C213" t="str">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214"/>
+      <c r="B214"/>
+      <c r="C214" t="str">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215"/>
+      <c r="B215"/>
+      <c r="C215" t="str">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216"/>
+      <c r="B216"/>
+      <c r="C216" t="str">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217"/>
+      <c r="B217"/>
+      <c r="C217" t="str">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218"/>
+      <c r="B218"/>
+      <c r="C218" t="str">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219"/>
+      <c r="B219"/>
+      <c r="C219" t="str">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220"/>
+      <c r="B220"/>
+      <c r="C220" t="str">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221"/>
+      <c r="B221"/>
+      <c r="C221" t="str">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222"/>
+      <c r="B222"/>
+      <c r="C222" t="str">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223"/>
+      <c r="B223"/>
+      <c r="C223" t="str">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224"/>
+      <c r="B224"/>
+      <c r="C224" t="str">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225"/>
+      <c r="B225"/>
+      <c r="C225" t="str">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226"/>
+      <c r="B226"/>
+      <c r="C226" t="str">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227"/>
+      <c r="B227"/>
+      <c r="C227" t="str">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228"/>
+      <c r="B228"/>
+      <c r="C228" t="str">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229"/>
+      <c r="B229"/>
+      <c r="C229" t="str">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230"/>
+      <c r="B230" t="str">
+        <v>10</v>
+      </c>
+      <c r="C230" t="str">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231"/>
+      <c r="B231"/>
+      <c r="C231" t="str">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232"/>
+      <c r="B232"/>
+      <c r="C232" t="str">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233"/>
+      <c r="B233"/>
+      <c r="C233" t="str">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234"/>
+      <c r="B234"/>
+      <c r="C234" t="str">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235"/>
+      <c r="B235"/>
+      <c r="C235" t="str">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236"/>
+      <c r="B236"/>
+      <c r="C236" t="str">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237"/>
+      <c r="B237"/>
+      <c r="C237" t="str">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238"/>
+      <c r="B238"/>
+      <c r="C238" t="str">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239"/>
+      <c r="B239"/>
+      <c r="C239" t="str">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240"/>
+      <c r="B240"/>
+      <c r="C240" t="str">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241"/>
+      <c r="B241"/>
+      <c r="C241" t="str">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242"/>
+      <c r="B242"/>
+      <c r="C242" t="str">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243"/>
+      <c r="B243"/>
+      <c r="C243" t="str">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244"/>
+      <c r="B244"/>
+      <c r="C244" t="str">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245"/>
+      <c r="B245"/>
+      <c r="C245" t="str">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246"/>
+      <c r="B246"/>
+      <c r="C246" t="str">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247"/>
+      <c r="B247"/>
+      <c r="C247" t="str">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248"/>
+      <c r="B248"/>
+      <c r="C248" t="str">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249"/>
+      <c r="B249"/>
+      <c r="C249" t="str">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250"/>
+      <c r="B250"/>
+      <c r="C250" t="str">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251"/>
+      <c r="B251"/>
+      <c r="C251" t="str">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252"/>
+      <c r="B252"/>
+      <c r="C252" t="str">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253"/>
+      <c r="B253"/>
+      <c r="C253" t="str">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254"/>
+      <c r="B254"/>
+      <c r="C254" t="str">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255"/>
+      <c r="B255"/>
+      <c r="C255" t="str">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256"/>
+      <c r="B256"/>
+      <c r="C256" t="str">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257"/>
+      <c r="B257"/>
+      <c r="C257" t="str">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258"/>
+      <c r="B258"/>
+      <c r="C258" t="str">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259"/>
+      <c r="B259"/>
+      <c r="C259" t="str">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260"/>
+      <c r="B260"/>
+      <c r="C260" t="str">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261"/>
+      <c r="B261"/>
+      <c r="C261" t="str">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262"/>
+      <c r="B262"/>
+      <c r="C262" t="str">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263"/>
+      <c r="B263"/>
+      <c r="C263" t="str">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264"/>
+      <c r="B264"/>
+      <c r="C264" t="str">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265"/>
+      <c r="B265"/>
+      <c r="C265" t="str">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266"/>
+      <c r="B266"/>
+      <c r="C266" t="str">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267"/>
+      <c r="B267"/>
+      <c r="C267" t="str">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268"/>
+      <c r="B268"/>
+      <c r="C268" t="str">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269"/>
+      <c r="B269"/>
+      <c r="C269" t="str">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270"/>
+      <c r="B270"/>
+      <c r="C270" t="str">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271"/>
+      <c r="B271"/>
+      <c r="C271" t="str">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272"/>
+      <c r="B272"/>
+      <c r="C272" t="str">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273"/>
+      <c r="B273"/>
+      <c r="C273" t="str">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274"/>
+      <c r="B274"/>
+      <c r="C274" t="str">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275"/>
+      <c r="B275"/>
+      <c r="C275" t="str">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276"/>
+      <c r="B276"/>
+      <c r="C276" t="str">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277"/>
+      <c r="B277"/>
+      <c r="C277" t="str">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278"/>
+      <c r="B278"/>
+      <c r="C278" t="str">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279"/>
+      <c r="B279"/>
+      <c r="C279" t="str">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280"/>
+      <c r="B280"/>
+      <c r="C280" t="str">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281"/>
+      <c r="B281"/>
+      <c r="C281" t="str">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282"/>
+      <c r="B282"/>
+      <c r="C282" t="str">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283"/>
+      <c r="B283"/>
+      <c r="C283" t="str">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284"/>
+      <c r="B284"/>
+      <c r="C284" t="str">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285"/>
+      <c r="B285"/>
+      <c r="C285" t="str">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286"/>
+      <c r="B286"/>
+      <c r="C286" t="str">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287"/>
+      <c r="B287"/>
+      <c r="C287" t="str">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288"/>
+      <c r="B288"/>
+      <c r="C288" t="str">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289"/>
+      <c r="B289"/>
+      <c r="C289" t="str">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290"/>
+      <c r="B290"/>
+      <c r="C290" t="str">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291"/>
+      <c r="B291"/>
+      <c r="C291" t="str">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292"/>
+      <c r="B292"/>
+      <c r="C292" t="str">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293"/>
+      <c r="B293"/>
+      <c r="C293" t="str">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294"/>
+      <c r="B294"/>
+      <c r="C294" t="str">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295"/>
+      <c r="B295"/>
+      <c r="C295" t="str">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296"/>
+      <c r="B296"/>
+      <c r="C296" t="str">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297"/>
+      <c r="B297"/>
+      <c r="C297" t="str">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298"/>
+      <c r="B298"/>
+      <c r="C298" t="str">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299"/>
+      <c r="B299"/>
+      <c r="C299" t="str">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300"/>
+      <c r="B300"/>
+      <c r="C300" t="str">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup scale="0" firstPageNumber="0" fitToWidth="0" fitToHeight="0" usePrinterDefaults="false" blackAndWhite="false" draft="false" useFirstPageNumber="false" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter differentFirst="false" differentOddEven="false"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
looping on row col functionality
</commit_message>
<xml_diff>
--- a/test/Workbook1.xlsx
+++ b/test/Workbook1.xlsx
@@ -1,29 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27417"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xuri/Sites/repo/excelize/test/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookPr date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="13220" yWindow="6260" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView activeTab="1" tabRatio="500" windowHeight="16880" windowWidth="28160" xWindow="13220" yWindow="6260"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="TestSheet" sheetId="3" r:id="rId6"/>
+    <sheet name="TestSheet" sheetId="3" r:id="rId7"/>
+    <sheet name="TestSheet" sheetId="3" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="150000"/>
+  <fileRecoveryPr repairLoad="0"/>
 </workbook>
 </file>
 
@@ -2442,14 +2435,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr filterMode="false"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="false" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="16"/>
   <sheetData>
     <row r="19" spans="2:2">
       <c r="A19" t="str">
@@ -2457,36 +2451,989 @@
       </c>
       <c r="B19">
         <f>SUM(Sheet2!D2,Sheet2!D11)</f>
-        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="false" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="0" firstPageNumber="0" fitToWidth="0" fitToHeight="0" usePrinterDefaults="false" blackAndWhite="false" draft="false" useFirstPageNumber="false" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter differentFirst="false" differentOddEven="false"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr filterMode="false"/>
+  <dimension ref=""/>
+  <sheetViews/>
+  <sheetFormatPr defaultRowHeight="0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+      <c r="B1"/>
+    </row>
+    <row r="2">
+      <c r="A2"/>
+      <c r="B2"/>
+    </row>
+    <row r="3">
+      <c r="A3"/>
+      <c r="B3"/>
+    </row>
+    <row r="4">
+      <c r="A4"/>
+      <c r="B4"/>
+    </row>
+    <row r="5">
+      <c r="A5"/>
+      <c r="B5"/>
+    </row>
+    <row r="6">
+      <c r="A6"/>
+      <c r="B6"/>
+    </row>
+    <row r="7">
+      <c r="A7"/>
+      <c r="B7"/>
+    </row>
+    <row r="8">
+      <c r="A8"/>
+      <c r="B8"/>
+    </row>
+    <row r="9">
+      <c r="A9"/>
+      <c r="B9"/>
+    </row>
+    <row r="10">
+      <c r="A10"/>
+      <c r="B10"/>
+    </row>
+    <row r="11">
+      <c r="A11"/>
+      <c r="B11"/>
+    </row>
+    <row r="12">
+      <c r="A12"/>
+      <c r="B12"/>
+    </row>
+    <row r="13">
+      <c r="A13"/>
+      <c r="B13"/>
+    </row>
+    <row r="14">
+      <c r="A14"/>
+      <c r="B14"/>
+    </row>
+    <row r="15">
+      <c r="A15"/>
+      <c r="B15"/>
+    </row>
+    <row r="16">
+      <c r="A16"/>
+      <c r="B16"/>
+    </row>
+    <row r="17">
+      <c r="A17"/>
+      <c r="B17"/>
+    </row>
+    <row r="18">
+      <c r="A18"/>
+      <c r="B18"/>
+    </row>
+    <row r="19">
+      <c r="A19"/>
+      <c r="B19"/>
+    </row>
+    <row r="20">
+      <c r="A20"/>
+      <c r="B20"/>
+    </row>
+    <row r="21">
+      <c r="A21"/>
+      <c r="B21"/>
+    </row>
+    <row r="22">
+      <c r="A22"/>
+      <c r="B22"/>
+    </row>
+    <row r="23">
+      <c r="A23"/>
+      <c r="B23"/>
+    </row>
+    <row r="24">
+      <c r="A24"/>
+      <c r="B24"/>
+    </row>
+    <row r="25">
+      <c r="A25"/>
+      <c r="B25"/>
+    </row>
+    <row r="26">
+      <c r="A26"/>
+      <c r="B26"/>
+    </row>
+    <row r="27">
+      <c r="A27"/>
+      <c r="B27"/>
+    </row>
+    <row r="28">
+      <c r="A28"/>
+      <c r="B28"/>
+    </row>
+    <row r="29">
+      <c r="A29"/>
+      <c r="B29"/>
+    </row>
+    <row r="30">
+      <c r="A30"/>
+      <c r="B30"/>
+    </row>
+    <row r="31">
+      <c r="A31"/>
+      <c r="B31"/>
+    </row>
+    <row r="32">
+      <c r="A32"/>
+      <c r="B32"/>
+    </row>
+    <row r="33">
+      <c r="A33"/>
+      <c r="B33"/>
+    </row>
+    <row r="34">
+      <c r="A34"/>
+      <c r="B34"/>
+    </row>
+    <row r="35">
+      <c r="A35"/>
+      <c r="B35"/>
+    </row>
+    <row r="36">
+      <c r="A36"/>
+      <c r="B36"/>
+    </row>
+    <row r="37">
+      <c r="A37"/>
+      <c r="B37"/>
+    </row>
+    <row r="38">
+      <c r="A38"/>
+      <c r="B38"/>
+    </row>
+    <row r="39">
+      <c r="A39"/>
+      <c r="B39"/>
+    </row>
+    <row r="40">
+      <c r="A40"/>
+      <c r="B40"/>
+    </row>
+    <row r="41">
+      <c r="A41"/>
+      <c r="B41"/>
+    </row>
+    <row r="42">
+      <c r="A42"/>
+      <c r="B42"/>
+    </row>
+    <row r="43">
+      <c r="A43"/>
+      <c r="B43"/>
+    </row>
+    <row r="44">
+      <c r="A44"/>
+      <c r="B44"/>
+    </row>
+    <row r="45">
+      <c r="A45"/>
+      <c r="B45"/>
+    </row>
+    <row r="46">
+      <c r="A46"/>
+      <c r="B46"/>
+    </row>
+    <row r="47">
+      <c r="A47"/>
+      <c r="B47"/>
+    </row>
+    <row r="48">
+      <c r="A48"/>
+      <c r="B48"/>
+    </row>
+    <row r="49">
+      <c r="A49"/>
+      <c r="B49"/>
+    </row>
+    <row r="50">
+      <c r="A50"/>
+      <c r="B50"/>
+    </row>
+    <row r="51">
+      <c r="A51"/>
+      <c r="B51"/>
+    </row>
+    <row r="52">
+      <c r="A52"/>
+      <c r="B52"/>
+    </row>
+    <row r="53">
+      <c r="A53"/>
+      <c r="B53"/>
+    </row>
+    <row r="54">
+      <c r="A54"/>
+      <c r="B54"/>
+    </row>
+    <row r="55">
+      <c r="A55"/>
+      <c r="B55"/>
+    </row>
+    <row r="56">
+      <c r="A56"/>
+      <c r="B56"/>
+    </row>
+    <row r="57">
+      <c r="A57"/>
+      <c r="B57"/>
+    </row>
+    <row r="58">
+      <c r="A58"/>
+      <c r="B58"/>
+    </row>
+    <row r="59">
+      <c r="A59"/>
+      <c r="B59"/>
+    </row>
+    <row r="60">
+      <c r="A60"/>
+      <c r="B60"/>
+    </row>
+    <row r="61">
+      <c r="A61"/>
+      <c r="B61"/>
+    </row>
+    <row r="62">
+      <c r="A62"/>
+      <c r="B62"/>
+    </row>
+    <row r="63">
+      <c r="A63"/>
+      <c r="B63"/>
+    </row>
+    <row r="64">
+      <c r="A64"/>
+      <c r="B64"/>
+    </row>
+    <row r="65">
+      <c r="A65"/>
+      <c r="B65"/>
+    </row>
+    <row r="66">
+      <c r="A66"/>
+      <c r="B66"/>
+    </row>
+    <row r="67">
+      <c r="A67"/>
+      <c r="B67"/>
+    </row>
+    <row r="68">
+      <c r="A68"/>
+      <c r="B68"/>
+    </row>
+    <row r="69">
+      <c r="A69"/>
+      <c r="B69"/>
+    </row>
+    <row r="70">
+      <c r="A70"/>
+      <c r="B70"/>
+    </row>
+    <row r="71">
+      <c r="A71"/>
+      <c r="B71"/>
+    </row>
+    <row r="72">
+      <c r="A72"/>
+      <c r="B72"/>
+    </row>
+    <row r="73">
+      <c r="A73"/>
+      <c r="B73"/>
+    </row>
+    <row r="74">
+      <c r="A74"/>
+      <c r="B74"/>
+    </row>
+    <row r="75">
+      <c r="A75"/>
+      <c r="B75"/>
+    </row>
+    <row r="76">
+      <c r="A76"/>
+      <c r="B76"/>
+    </row>
+    <row r="77">
+      <c r="A77"/>
+      <c r="B77"/>
+    </row>
+    <row r="78">
+      <c r="A78"/>
+      <c r="B78"/>
+    </row>
+    <row r="79">
+      <c r="A79"/>
+      <c r="B79"/>
+    </row>
+    <row r="80">
+      <c r="A80"/>
+      <c r="B80"/>
+    </row>
+    <row r="81">
+      <c r="A81"/>
+      <c r="B81"/>
+    </row>
+    <row r="82">
+      <c r="A82"/>
+      <c r="B82"/>
+    </row>
+    <row r="83">
+      <c r="A83"/>
+      <c r="B83"/>
+    </row>
+    <row r="84">
+      <c r="A84"/>
+      <c r="B84"/>
+    </row>
+    <row r="85">
+      <c r="A85"/>
+      <c r="B85"/>
+    </row>
+    <row r="86">
+      <c r="A86"/>
+      <c r="B86"/>
+    </row>
+    <row r="87">
+      <c r="A87"/>
+      <c r="B87"/>
+    </row>
+    <row r="88">
+      <c r="A88"/>
+      <c r="B88"/>
+    </row>
+    <row r="89">
+      <c r="A89"/>
+      <c r="B89"/>
+    </row>
+    <row r="90">
+      <c r="A90"/>
+      <c r="B90"/>
+    </row>
+    <row r="91">
+      <c r="A91"/>
+      <c r="B91"/>
+    </row>
+    <row r="92">
+      <c r="A92"/>
+      <c r="B92"/>
+    </row>
+    <row r="93">
+      <c r="A93"/>
+      <c r="B93"/>
+    </row>
+    <row r="94">
+      <c r="A94"/>
+      <c r="B94"/>
+    </row>
+    <row r="95">
+      <c r="A95"/>
+      <c r="B95"/>
+    </row>
+    <row r="96">
+      <c r="A96"/>
+      <c r="B96"/>
+    </row>
+    <row r="97">
+      <c r="A97"/>
+      <c r="B97"/>
+    </row>
+    <row r="98">
+      <c r="A98"/>
+      <c r="B98"/>
+    </row>
+    <row r="99">
+      <c r="A99"/>
+      <c r="B99"/>
+    </row>
+    <row r="100">
+      <c r="A100"/>
+      <c r="B100"/>
+    </row>
+    <row r="101">
+      <c r="A101"/>
+      <c r="B101"/>
+    </row>
+    <row r="102">
+      <c r="A102"/>
+      <c r="B102"/>
+    </row>
+    <row r="103">
+      <c r="A103"/>
+      <c r="B103"/>
+    </row>
+    <row r="104">
+      <c r="A104"/>
+      <c r="B104"/>
+    </row>
+    <row r="105">
+      <c r="A105"/>
+      <c r="B105"/>
+    </row>
+    <row r="106">
+      <c r="A106"/>
+      <c r="B106"/>
+    </row>
+    <row r="107">
+      <c r="A107"/>
+      <c r="B107"/>
+    </row>
+    <row r="108">
+      <c r="A108"/>
+      <c r="B108"/>
+    </row>
+    <row r="109">
+      <c r="A109"/>
+      <c r="B109"/>
+    </row>
+    <row r="110">
+      <c r="A110"/>
+      <c r="B110"/>
+    </row>
+    <row r="111">
+      <c r="A111"/>
+      <c r="B111"/>
+    </row>
+    <row r="112">
+      <c r="A112"/>
+      <c r="B112"/>
+    </row>
+    <row r="113">
+      <c r="A113"/>
+      <c r="B113"/>
+    </row>
+    <row r="114">
+      <c r="A114"/>
+      <c r="B114"/>
+    </row>
+    <row r="115">
+      <c r="A115"/>
+      <c r="B115"/>
+    </row>
+    <row r="116">
+      <c r="A116"/>
+      <c r="B116"/>
+    </row>
+    <row r="117">
+      <c r="A117"/>
+      <c r="B117"/>
+    </row>
+    <row r="118">
+      <c r="A118"/>
+      <c r="B118"/>
+    </row>
+    <row r="119">
+      <c r="A119"/>
+      <c r="B119"/>
+    </row>
+    <row r="120">
+      <c r="A120"/>
+      <c r="B120"/>
+    </row>
+    <row r="121">
+      <c r="A121"/>
+      <c r="B121"/>
+    </row>
+    <row r="122">
+      <c r="A122"/>
+      <c r="B122"/>
+    </row>
+    <row r="123">
+      <c r="A123"/>
+      <c r="B123"/>
+    </row>
+    <row r="124">
+      <c r="A124"/>
+      <c r="B124"/>
+    </row>
+    <row r="125">
+      <c r="A125"/>
+      <c r="B125"/>
+    </row>
+    <row r="126">
+      <c r="A126"/>
+      <c r="B126"/>
+    </row>
+    <row r="127">
+      <c r="A127"/>
+      <c r="B127"/>
+    </row>
+    <row r="128">
+      <c r="A128"/>
+      <c r="B128"/>
+    </row>
+    <row r="129">
+      <c r="A129"/>
+      <c r="B129"/>
+    </row>
+    <row r="130">
+      <c r="A130"/>
+      <c r="B130"/>
+    </row>
+    <row r="131">
+      <c r="A131"/>
+      <c r="B131"/>
+    </row>
+    <row r="132">
+      <c r="A132"/>
+      <c r="B132"/>
+    </row>
+    <row r="133">
+      <c r="A133"/>
+      <c r="B133"/>
+    </row>
+    <row r="134">
+      <c r="A134"/>
+      <c r="B134"/>
+    </row>
+    <row r="135">
+      <c r="A135"/>
+      <c r="B135"/>
+    </row>
+    <row r="136">
+      <c r="A136"/>
+      <c r="B136"/>
+    </row>
+    <row r="137">
+      <c r="A137"/>
+      <c r="B137"/>
+    </row>
+    <row r="138">
+      <c r="A138"/>
+      <c r="B138"/>
+    </row>
+    <row r="139">
+      <c r="A139"/>
+      <c r="B139"/>
+    </row>
+    <row r="140">
+      <c r="A140"/>
+      <c r="B140"/>
+    </row>
+    <row r="141">
+      <c r="A141"/>
+      <c r="B141"/>
+    </row>
+    <row r="142">
+      <c r="A142"/>
+      <c r="B142"/>
+    </row>
+    <row r="143">
+      <c r="A143"/>
+      <c r="B143"/>
+    </row>
+    <row r="144">
+      <c r="A144"/>
+      <c r="B144"/>
+    </row>
+    <row r="145">
+      <c r="A145"/>
+      <c r="B145"/>
+    </row>
+    <row r="146">
+      <c r="A146"/>
+      <c r="B146"/>
+    </row>
+    <row r="147">
+      <c r="A147"/>
+      <c r="B147"/>
+    </row>
+    <row r="148">
+      <c r="A148"/>
+      <c r="B148"/>
+    </row>
+    <row r="149">
+      <c r="A149"/>
+      <c r="B149"/>
+    </row>
+    <row r="150">
+      <c r="A150"/>
+      <c r="B150"/>
+    </row>
+    <row r="151">
+      <c r="A151"/>
+      <c r="B151"/>
+    </row>
+    <row r="152">
+      <c r="A152"/>
+      <c r="B152"/>
+    </row>
+    <row r="153">
+      <c r="A153"/>
+      <c r="B153"/>
+    </row>
+    <row r="154">
+      <c r="A154"/>
+      <c r="B154"/>
+    </row>
+    <row r="155">
+      <c r="A155"/>
+      <c r="B155"/>
+    </row>
+    <row r="156">
+      <c r="A156"/>
+      <c r="B156"/>
+    </row>
+    <row r="157">
+      <c r="A157"/>
+      <c r="B157"/>
+    </row>
+    <row r="158">
+      <c r="A158"/>
+      <c r="B158"/>
+    </row>
+    <row r="159">
+      <c r="A159"/>
+      <c r="B159"/>
+    </row>
+    <row r="160">
+      <c r="A160"/>
+      <c r="B160"/>
+    </row>
+    <row r="161">
+      <c r="A161"/>
+      <c r="B161"/>
+    </row>
+    <row r="162">
+      <c r="A162"/>
+      <c r="B162"/>
+    </row>
+    <row r="163">
+      <c r="A163"/>
+      <c r="B163"/>
+    </row>
+    <row r="164">
+      <c r="A164"/>
+      <c r="B164"/>
+    </row>
+    <row r="165">
+      <c r="A165"/>
+      <c r="B165"/>
+    </row>
+    <row r="166">
+      <c r="A166"/>
+      <c r="B166"/>
+    </row>
+    <row r="167">
+      <c r="A167"/>
+      <c r="B167"/>
+    </row>
+    <row r="168">
+      <c r="A168"/>
+      <c r="B168"/>
+    </row>
+    <row r="169">
+      <c r="A169"/>
+      <c r="B169"/>
+    </row>
+    <row r="170">
+      <c r="A170"/>
+      <c r="B170"/>
+    </row>
+    <row r="171">
+      <c r="A171"/>
+      <c r="B171"/>
+    </row>
+    <row r="172">
+      <c r="A172"/>
+      <c r="B172"/>
+    </row>
+    <row r="173">
+      <c r="A173"/>
+      <c r="B173"/>
+    </row>
+    <row r="174">
+      <c r="A174"/>
+      <c r="B174"/>
+    </row>
+    <row r="175">
+      <c r="A175"/>
+      <c r="B175"/>
+    </row>
+    <row r="176">
+      <c r="A176"/>
+      <c r="B176"/>
+    </row>
+    <row r="177">
+      <c r="A177"/>
+      <c r="B177"/>
+    </row>
+    <row r="178">
+      <c r="A178"/>
+      <c r="B178"/>
+    </row>
+    <row r="179">
+      <c r="A179"/>
+      <c r="B179"/>
+    </row>
+    <row r="180">
+      <c r="A180"/>
+      <c r="B180"/>
+    </row>
+    <row r="181">
+      <c r="A181"/>
+      <c r="B181"/>
+    </row>
+    <row r="182">
+      <c r="A182"/>
+      <c r="B182"/>
+    </row>
+    <row r="183">
+      <c r="A183"/>
+      <c r="B183"/>
+    </row>
+    <row r="184">
+      <c r="A184"/>
+      <c r="B184"/>
+    </row>
+    <row r="185">
+      <c r="A185"/>
+      <c r="B185"/>
+    </row>
+    <row r="186">
+      <c r="A186"/>
+      <c r="B186"/>
+    </row>
+    <row r="187">
+      <c r="A187"/>
+      <c r="B187"/>
+    </row>
+    <row r="188">
+      <c r="A188"/>
+      <c r="B188"/>
+    </row>
+    <row r="189">
+      <c r="A189"/>
+      <c r="B189"/>
+    </row>
+    <row r="190">
+      <c r="A190"/>
+      <c r="B190"/>
+    </row>
+    <row r="191">
+      <c r="A191"/>
+      <c r="B191"/>
+    </row>
+    <row r="192">
+      <c r="A192"/>
+      <c r="B192"/>
+    </row>
+    <row r="193">
+      <c r="A193"/>
+      <c r="B193"/>
+    </row>
+    <row r="194">
+      <c r="A194"/>
+      <c r="B194"/>
+    </row>
+    <row r="195">
+      <c r="A195"/>
+      <c r="B195"/>
+    </row>
+    <row r="196">
+      <c r="A196"/>
+      <c r="B196"/>
+    </row>
+    <row r="197">
+      <c r="A197"/>
+      <c r="B197"/>
+    </row>
+    <row r="198">
+      <c r="A198"/>
+      <c r="B198"/>
+    </row>
+    <row r="199">
+      <c r="A199"/>
+      <c r="B199"/>
+    </row>
+    <row r="200">
+      <c r="A200"/>
+      <c r="B200"/>
+    </row>
+    <row r="201">
+      <c r="A201"/>
+      <c r="B201"/>
+    </row>
+    <row r="202">
+      <c r="A202"/>
+      <c r="B202"/>
+    </row>
+    <row r="203">
+      <c r="A203"/>
+      <c r="B203"/>
+    </row>
+    <row r="204">
+      <c r="A204"/>
+      <c r="B204"/>
+    </row>
+    <row r="205">
+      <c r="A205"/>
+      <c r="B205"/>
+    </row>
+    <row r="206">
+      <c r="A206"/>
+      <c r="B206"/>
+    </row>
+    <row r="207">
+      <c r="A207"/>
+      <c r="B207"/>
+    </row>
+    <row r="208">
+      <c r="A208"/>
+      <c r="B208"/>
+    </row>
+    <row r="209">
+      <c r="A209"/>
+      <c r="B209"/>
+    </row>
+    <row r="210">
+      <c r="A210"/>
+      <c r="B210"/>
+    </row>
+    <row r="211">
+      <c r="A211"/>
+      <c r="B211"/>
+    </row>
+    <row r="212">
+      <c r="A212"/>
+      <c r="B212"/>
+    </row>
+    <row r="213">
+      <c r="A213"/>
+      <c r="B213"/>
+    </row>
+    <row r="214">
+      <c r="A214"/>
+      <c r="B214"/>
+    </row>
+    <row r="215">
+      <c r="A215"/>
+      <c r="B215"/>
+    </row>
+    <row r="216">
+      <c r="A216"/>
+      <c r="B216"/>
+    </row>
+    <row r="217">
+      <c r="A217"/>
+      <c r="B217"/>
+    </row>
+    <row r="218">
+      <c r="A218"/>
+      <c r="B218"/>
+    </row>
+    <row r="219">
+      <c r="A219"/>
+      <c r="B219"/>
+    </row>
+    <row r="220">
+      <c r="A220"/>
+      <c r="B220"/>
+    </row>
+    <row r="221">
+      <c r="A221"/>
+      <c r="B221"/>
+    </row>
+    <row r="222">
+      <c r="A222"/>
+      <c r="B222"/>
+    </row>
+    <row r="223">
+      <c r="A223"/>
+      <c r="B223"/>
+    </row>
+    <row r="224">
+      <c r="A224"/>
+      <c r="B224"/>
+    </row>
+    <row r="225">
+      <c r="A225"/>
+      <c r="B225"/>
+    </row>
+    <row r="226">
+      <c r="A226"/>
+      <c r="B226"/>
+    </row>
+    <row r="227">
+      <c r="A227"/>
+      <c r="B227"/>
+    </row>
+    <row r="228">
+      <c r="A228"/>
+      <c r="B228"/>
+    </row>
+    <row r="229">
+      <c r="A229"/>
+      <c r="B229"/>
+    </row>
+    <row r="230">
+      <c r="A230"/>
+      <c r="B230" t="str">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup scale="0" firstPageNumber="0" fitToWidth="0" fitToHeight="0" usePrinterDefaults="false" blackAndWhite="false" draft="false" useFirstPageNumber="false" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter differentFirst="false" differentOddEven="false"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr filterMode="false"/>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
+    <row r="1" spans="1:4" ht="17">
+      <c r="A1" s="1">
+        <v>100</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E1"/>
+      <c r="F1" t="str">
+        <v>Hello</v>
+      </c>
+      <c r="G1" t="str">
+        <v>World</v>
+      </c>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1"/>
+      <c r="L1"/>
+      <c r="M1"/>
+    </row>
+    <row r="2" spans="1:4" ht="17">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -2499,8 +3446,19 @@
       <c r="D2" s="4">
         <v>200</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E2"/>
+      <c r="F2">
+        <v>42</v>
+      </c>
+      <c r="G2" t="str"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2" t="str"/>
+    </row>
+    <row r="3" spans="1:4" ht="17">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2513,8 +3471,17 @@
       <c r="D3" s="4">
         <v>450</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+    </row>
+    <row r="4" spans="1:4" ht="17">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -2527,8 +3494,17 @@
       <c r="D4" s="4">
         <v>200</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+    </row>
+    <row r="5" spans="1:4" ht="17">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -2541,57 +3517,2313 @@
       <c r="D5" s="4">
         <v>510</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6"/>
+      <c r="B6"/>
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="4">
         <v>315</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7"/>
+      <c r="B7"/>
       <c r="C7" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="4">
         <v>127</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8"/>
+      <c r="B8"/>
       <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="4">
         <v>89</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9"/>
+      <c r="B9"/>
       <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="4">
         <v>348</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10"/>
+      <c r="B10"/>
       <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="4">
         <v>53</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11"/>
+      <c r="B11"/>
       <c r="C11" s="4" t="str">
-        <v>Other</v>
+        <v>Knowns</v>
       </c>
       <c r="D11" s="4">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+    </row>
+    <row r="13">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+    </row>
   </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="false" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="0" firstPageNumber="0" fitToWidth="0" fitToHeight="0" usePrinterDefaults="false" blackAndWhite="false" draft="false" useFirstPageNumber="false" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter differentFirst="false" differentOddEven="false"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr filterMode="false"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="false" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+      <c r="B1"/>
+      <c r="C1" t="str">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2" t="str">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="C3" t="str">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4" t="str">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6" t="str">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7" t="str">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8" t="str">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9" t="str">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10" t="str">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11" t="str">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12" t="str">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13" t="str">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14" t="str">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15" t="str">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16" t="str">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17" t="str">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18" t="str">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19" t="str">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20" t="str">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21" t="str">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22" t="str">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>10</v>
+      </c>
+      <c r="B23"/>
+      <c r="C23" t="str">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24" t="str">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25" t="str">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26" t="str">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27" t="str">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28" t="str">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29" t="str">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30"/>
+      <c r="B30"/>
+      <c r="C30" t="str">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31" t="str">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32"/>
+      <c r="B32"/>
+      <c r="C32" t="str">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33"/>
+      <c r="B33"/>
+      <c r="C33" t="str">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34" t="str">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35"/>
+      <c r="B35"/>
+      <c r="C35" t="str">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36"/>
+      <c r="B36"/>
+      <c r="C36" t="str">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37"/>
+      <c r="B37"/>
+      <c r="C37" t="str">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38"/>
+      <c r="B38"/>
+      <c r="C38" t="str">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39"/>
+      <c r="B39"/>
+      <c r="C39" t="str">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40"/>
+      <c r="B40"/>
+      <c r="C40" t="str">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41"/>
+      <c r="B41"/>
+      <c r="C41" t="str">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42"/>
+      <c r="B42"/>
+      <c r="C42" t="str">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43"/>
+      <c r="B43"/>
+      <c r="C43" t="str">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44"/>
+      <c r="B44"/>
+      <c r="C44" t="str">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45"/>
+      <c r="B45"/>
+      <c r="C45" t="str">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46"/>
+      <c r="B46"/>
+      <c r="C46" t="str">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47"/>
+      <c r="B47"/>
+      <c r="C47" t="str">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48"/>
+      <c r="B48"/>
+      <c r="C48" t="str">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49"/>
+      <c r="B49"/>
+      <c r="C49" t="str">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50"/>
+      <c r="B50"/>
+      <c r="C50" t="str">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51"/>
+      <c r="B51"/>
+      <c r="C51" t="str">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52"/>
+      <c r="B52"/>
+      <c r="C52" t="str">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53"/>
+      <c r="B53"/>
+      <c r="C53" t="str">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54"/>
+      <c r="B54"/>
+      <c r="C54" t="str">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55"/>
+      <c r="B55"/>
+      <c r="C55" t="str">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56"/>
+      <c r="B56"/>
+      <c r="C56" t="str">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57"/>
+      <c r="B57"/>
+      <c r="C57" t="str">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58"/>
+      <c r="B58"/>
+      <c r="C58" t="str">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59"/>
+      <c r="B59"/>
+      <c r="C59" t="str">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60"/>
+      <c r="B60"/>
+      <c r="C60" t="str">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61"/>
+      <c r="B61"/>
+      <c r="C61" t="str">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62"/>
+      <c r="B62"/>
+      <c r="C62" t="str">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63"/>
+      <c r="B63"/>
+      <c r="C63" t="str">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64"/>
+      <c r="B64"/>
+      <c r="C64" t="str">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65"/>
+      <c r="B65"/>
+      <c r="C65" t="str">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66"/>
+      <c r="B66"/>
+      <c r="C66" t="str">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67"/>
+      <c r="B67"/>
+      <c r="C67" t="str">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68"/>
+      <c r="B68"/>
+      <c r="C68" t="str">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69"/>
+      <c r="B69"/>
+      <c r="C69" t="str">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70"/>
+      <c r="B70"/>
+      <c r="C70" t="str">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71"/>
+      <c r="B71"/>
+      <c r="C71" t="str">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72"/>
+      <c r="B72"/>
+      <c r="C72" t="str">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73"/>
+      <c r="B73"/>
+      <c r="C73" t="str">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74"/>
+      <c r="B74"/>
+      <c r="C74" t="str">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75"/>
+      <c r="B75"/>
+      <c r="C75" t="str">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76"/>
+      <c r="B76"/>
+      <c r="C76" t="str">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77"/>
+      <c r="B77"/>
+      <c r="C77" t="str">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78"/>
+      <c r="B78"/>
+      <c r="C78" t="str">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79"/>
+      <c r="B79"/>
+      <c r="C79" t="str">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80"/>
+      <c r="B80"/>
+      <c r="C80" t="str">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81"/>
+      <c r="B81"/>
+      <c r="C81" t="str">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82"/>
+      <c r="B82"/>
+      <c r="C82" t="str">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83"/>
+      <c r="B83"/>
+      <c r="C83" t="str">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84"/>
+      <c r="B84"/>
+      <c r="C84" t="str">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85"/>
+      <c r="B85"/>
+      <c r="C85" t="str">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86"/>
+      <c r="B86"/>
+      <c r="C86" t="str">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87"/>
+      <c r="B87"/>
+      <c r="C87" t="str">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88"/>
+      <c r="B88"/>
+      <c r="C88" t="str">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89"/>
+      <c r="B89"/>
+      <c r="C89" t="str">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90"/>
+      <c r="B90"/>
+      <c r="C90" t="str">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91"/>
+      <c r="B91"/>
+      <c r="C91" t="str">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92"/>
+      <c r="B92"/>
+      <c r="C92" t="str">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93"/>
+      <c r="B93"/>
+      <c r="C93" t="str">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94"/>
+      <c r="B94"/>
+      <c r="C94" t="str">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95"/>
+      <c r="B95"/>
+      <c r="C95" t="str">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96"/>
+      <c r="B96"/>
+      <c r="C96" t="str">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97"/>
+      <c r="B97"/>
+      <c r="C97" t="str">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98"/>
+      <c r="B98"/>
+      <c r="C98" t="str">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99"/>
+      <c r="B99"/>
+      <c r="C99" t="str">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100"/>
+      <c r="B100"/>
+      <c r="C100" t="str">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101"/>
+      <c r="B101"/>
+      <c r="C101" t="str">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102"/>
+      <c r="B102"/>
+      <c r="C102" t="str">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103"/>
+      <c r="B103"/>
+      <c r="C103" t="str">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104"/>
+      <c r="B104"/>
+      <c r="C104" t="str">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105"/>
+      <c r="B105"/>
+      <c r="C105" t="str">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106"/>
+      <c r="B106"/>
+      <c r="C106" t="str">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107"/>
+      <c r="B107"/>
+      <c r="C107" t="str">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108"/>
+      <c r="B108"/>
+      <c r="C108" t="str">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109"/>
+      <c r="B109"/>
+      <c r="C109" t="str">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110"/>
+      <c r="B110"/>
+      <c r="C110" t="str">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111"/>
+      <c r="B111"/>
+      <c r="C111" t="str">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112"/>
+      <c r="B112"/>
+      <c r="C112" t="str">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113"/>
+      <c r="B113"/>
+      <c r="C113" t="str">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114"/>
+      <c r="B114"/>
+      <c r="C114" t="str">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115"/>
+      <c r="B115"/>
+      <c r="C115" t="str">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116"/>
+      <c r="B116"/>
+      <c r="C116" t="str">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117"/>
+      <c r="B117"/>
+      <c r="C117" t="str">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118"/>
+      <c r="B118"/>
+      <c r="C118" t="str">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119"/>
+      <c r="B119"/>
+      <c r="C119" t="str">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120"/>
+      <c r="B120"/>
+      <c r="C120" t="str">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121"/>
+      <c r="B121"/>
+      <c r="C121" t="str">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122"/>
+      <c r="B122"/>
+      <c r="C122" t="str">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123"/>
+      <c r="B123"/>
+      <c r="C123" t="str">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124"/>
+      <c r="B124"/>
+      <c r="C124" t="str">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125"/>
+      <c r="B125"/>
+      <c r="C125" t="str">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126"/>
+      <c r="B126"/>
+      <c r="C126" t="str">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127"/>
+      <c r="B127"/>
+      <c r="C127" t="str">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128"/>
+      <c r="B128"/>
+      <c r="C128" t="str">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129"/>
+      <c r="B129"/>
+      <c r="C129" t="str">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130"/>
+      <c r="B130"/>
+      <c r="C130" t="str">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131"/>
+      <c r="B131"/>
+      <c r="C131" t="str">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132"/>
+      <c r="B132"/>
+      <c r="C132" t="str">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133"/>
+      <c r="B133"/>
+      <c r="C133" t="str">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134"/>
+      <c r="B134"/>
+      <c r="C134" t="str">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135"/>
+      <c r="B135"/>
+      <c r="C135" t="str">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136"/>
+      <c r="B136"/>
+      <c r="C136" t="str">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137"/>
+      <c r="B137"/>
+      <c r="C137" t="str">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138"/>
+      <c r="B138"/>
+      <c r="C138" t="str">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139"/>
+      <c r="B139"/>
+      <c r="C139" t="str">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140"/>
+      <c r="B140"/>
+      <c r="C140" t="str">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141"/>
+      <c r="B141"/>
+      <c r="C141" t="str">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142"/>
+      <c r="B142"/>
+      <c r="C142" t="str">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143"/>
+      <c r="B143"/>
+      <c r="C143" t="str">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144"/>
+      <c r="B144"/>
+      <c r="C144" t="str">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145"/>
+      <c r="B145"/>
+      <c r="C145" t="str">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146"/>
+      <c r="B146"/>
+      <c r="C146" t="str">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147"/>
+      <c r="B147"/>
+      <c r="C147" t="str">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148"/>
+      <c r="B148"/>
+      <c r="C148" t="str">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149"/>
+      <c r="B149"/>
+      <c r="C149" t="str">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150"/>
+      <c r="B150"/>
+      <c r="C150" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151"/>
+      <c r="B151"/>
+      <c r="C151" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152"/>
+      <c r="B152"/>
+      <c r="C152" t="str">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153"/>
+      <c r="B153"/>
+      <c r="C153" t="str">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154"/>
+      <c r="B154"/>
+      <c r="C154" t="str">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155"/>
+      <c r="B155"/>
+      <c r="C155" t="str">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156"/>
+      <c r="B156"/>
+      <c r="C156" t="str">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157"/>
+      <c r="B157"/>
+      <c r="C157" t="str">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158"/>
+      <c r="B158"/>
+      <c r="C158" t="str">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159"/>
+      <c r="B159"/>
+      <c r="C159" t="str">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160"/>
+      <c r="B160"/>
+      <c r="C160" t="str">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161"/>
+      <c r="B161"/>
+      <c r="C161" t="str">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162"/>
+      <c r="B162"/>
+      <c r="C162" t="str">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163"/>
+      <c r="B163"/>
+      <c r="C163" t="str">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164"/>
+      <c r="B164"/>
+      <c r="C164" t="str">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165"/>
+      <c r="B165"/>
+      <c r="C165" t="str">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166"/>
+      <c r="B166"/>
+      <c r="C166" t="str">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167"/>
+      <c r="B167"/>
+      <c r="C167" t="str">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168"/>
+      <c r="B168"/>
+      <c r="C168" t="str">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169"/>
+      <c r="B169"/>
+      <c r="C169" t="str">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170"/>
+      <c r="B170"/>
+      <c r="C170" t="str">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171"/>
+      <c r="B171"/>
+      <c r="C171" t="str">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172"/>
+      <c r="B172"/>
+      <c r="C172" t="str">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173"/>
+      <c r="B173"/>
+      <c r="C173" t="str">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174"/>
+      <c r="B174"/>
+      <c r="C174" t="str">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175"/>
+      <c r="B175"/>
+      <c r="C175" t="str">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176"/>
+      <c r="B176"/>
+      <c r="C176" t="str">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177"/>
+      <c r="B177"/>
+      <c r="C177" t="str">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178"/>
+      <c r="B178"/>
+      <c r="C178" t="str">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179"/>
+      <c r="B179"/>
+      <c r="C179" t="str">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180"/>
+      <c r="B180"/>
+      <c r="C180" t="str">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181"/>
+      <c r="B181"/>
+      <c r="C181" t="str">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182"/>
+      <c r="B182"/>
+      <c r="C182" t="str">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183"/>
+      <c r="B183"/>
+      <c r="C183" t="str">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184"/>
+      <c r="B184"/>
+      <c r="C184" t="str">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185"/>
+      <c r="B185"/>
+      <c r="C185" t="str">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186"/>
+      <c r="B186"/>
+      <c r="C186" t="str">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187"/>
+      <c r="B187"/>
+      <c r="C187" t="str">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188"/>
+      <c r="B188"/>
+      <c r="C188" t="str">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189"/>
+      <c r="B189"/>
+      <c r="C189" t="str">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190"/>
+      <c r="B190"/>
+      <c r="C190" t="str">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191"/>
+      <c r="B191"/>
+      <c r="C191" t="str">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192"/>
+      <c r="B192"/>
+      <c r="C192" t="str">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193"/>
+      <c r="B193"/>
+      <c r="C193" t="str">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194"/>
+      <c r="B194"/>
+      <c r="C194" t="str">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195"/>
+      <c r="B195"/>
+      <c r="C195" t="str">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196"/>
+      <c r="B196"/>
+      <c r="C196" t="str">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197"/>
+      <c r="B197"/>
+      <c r="C197" t="str">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198"/>
+      <c r="B198"/>
+      <c r="C198" t="str">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199"/>
+      <c r="B199"/>
+      <c r="C199" t="str">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200"/>
+      <c r="B200"/>
+      <c r="C200" t="str">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201"/>
+      <c r="B201"/>
+      <c r="C201" t="str">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202"/>
+      <c r="B202"/>
+      <c r="C202" t="str">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203"/>
+      <c r="B203"/>
+      <c r="C203" t="str">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204"/>
+      <c r="B204"/>
+      <c r="C204" t="str">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205"/>
+      <c r="B205"/>
+      <c r="C205" t="str">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206"/>
+      <c r="B206"/>
+      <c r="C206" t="str">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207"/>
+      <c r="B207"/>
+      <c r="C207" t="str">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208"/>
+      <c r="B208"/>
+      <c r="C208" t="str">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209"/>
+      <c r="B209"/>
+      <c r="C209" t="str">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210"/>
+      <c r="B210"/>
+      <c r="C210" t="str">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211"/>
+      <c r="B211"/>
+      <c r="C211" t="str">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212"/>
+      <c r="B212"/>
+      <c r="C212" t="str">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213"/>
+      <c r="B213"/>
+      <c r="C213" t="str">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214"/>
+      <c r="B214"/>
+      <c r="C214" t="str">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215"/>
+      <c r="B215"/>
+      <c r="C215" t="str">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216"/>
+      <c r="B216"/>
+      <c r="C216" t="str">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217"/>
+      <c r="B217"/>
+      <c r="C217" t="str">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218"/>
+      <c r="B218"/>
+      <c r="C218" t="str">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219"/>
+      <c r="B219"/>
+      <c r="C219" t="str">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220"/>
+      <c r="B220"/>
+      <c r="C220" t="str">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221"/>
+      <c r="B221"/>
+      <c r="C221" t="str">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222"/>
+      <c r="B222"/>
+      <c r="C222" t="str">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223"/>
+      <c r="B223"/>
+      <c r="C223" t="str">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224"/>
+      <c r="B224"/>
+      <c r="C224" t="str">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225"/>
+      <c r="B225"/>
+      <c r="C225" t="str">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226"/>
+      <c r="B226"/>
+      <c r="C226" t="str">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227"/>
+      <c r="B227"/>
+      <c r="C227" t="str">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228"/>
+      <c r="B228"/>
+      <c r="C228" t="str">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229"/>
+      <c r="B229"/>
+      <c r="C229" t="str">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230"/>
+      <c r="B230" t="str">
+        <v>10</v>
+      </c>
+      <c r="C230" t="str">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231"/>
+      <c r="B231"/>
+      <c r="C231" t="str">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232"/>
+      <c r="B232"/>
+      <c r="C232" t="str">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233"/>
+      <c r="B233"/>
+      <c r="C233" t="str">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234"/>
+      <c r="B234"/>
+      <c r="C234" t="str">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235"/>
+      <c r="B235"/>
+      <c r="C235" t="str">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236"/>
+      <c r="B236"/>
+      <c r="C236" t="str">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237"/>
+      <c r="B237"/>
+      <c r="C237" t="str">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238"/>
+      <c r="B238"/>
+      <c r="C238" t="str">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239"/>
+      <c r="B239"/>
+      <c r="C239" t="str">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240"/>
+      <c r="B240"/>
+      <c r="C240" t="str">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241"/>
+      <c r="B241"/>
+      <c r="C241" t="str">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242"/>
+      <c r="B242"/>
+      <c r="C242" t="str">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243"/>
+      <c r="B243"/>
+      <c r="C243" t="str">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244"/>
+      <c r="B244"/>
+      <c r="C244" t="str">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245"/>
+      <c r="B245"/>
+      <c r="C245" t="str">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246"/>
+      <c r="B246"/>
+      <c r="C246" t="str">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247"/>
+      <c r="B247"/>
+      <c r="C247" t="str">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248"/>
+      <c r="B248"/>
+      <c r="C248" t="str">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249"/>
+      <c r="B249"/>
+      <c r="C249" t="str">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250"/>
+      <c r="B250"/>
+      <c r="C250" t="str">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251"/>
+      <c r="B251"/>
+      <c r="C251" t="str">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252"/>
+      <c r="B252"/>
+      <c r="C252" t="str">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253"/>
+      <c r="B253"/>
+      <c r="C253" t="str">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254"/>
+      <c r="B254"/>
+      <c r="C254" t="str">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255"/>
+      <c r="B255"/>
+      <c r="C255" t="str">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256"/>
+      <c r="B256"/>
+      <c r="C256" t="str">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257"/>
+      <c r="B257"/>
+      <c r="C257" t="str">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258"/>
+      <c r="B258"/>
+      <c r="C258" t="str">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259"/>
+      <c r="B259"/>
+      <c r="C259" t="str">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260"/>
+      <c r="B260"/>
+      <c r="C260" t="str">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261"/>
+      <c r="B261"/>
+      <c r="C261" t="str">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262"/>
+      <c r="B262"/>
+      <c r="C262" t="str">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263"/>
+      <c r="B263"/>
+      <c r="C263" t="str">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264"/>
+      <c r="B264"/>
+      <c r="C264" t="str">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265"/>
+      <c r="B265"/>
+      <c r="C265" t="str">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266"/>
+      <c r="B266"/>
+      <c r="C266" t="str">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267"/>
+      <c r="B267"/>
+      <c r="C267" t="str">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268"/>
+      <c r="B268"/>
+      <c r="C268" t="str">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269"/>
+      <c r="B269"/>
+      <c r="C269" t="str">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270"/>
+      <c r="B270"/>
+      <c r="C270" t="str">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271"/>
+      <c r="B271"/>
+      <c r="C271" t="str">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272"/>
+      <c r="B272"/>
+      <c r="C272" t="str">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273"/>
+      <c r="B273"/>
+      <c r="C273" t="str">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274"/>
+      <c r="B274"/>
+      <c r="C274" t="str">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275"/>
+      <c r="B275"/>
+      <c r="C275" t="str">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276"/>
+      <c r="B276"/>
+      <c r="C276" t="str">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277"/>
+      <c r="B277"/>
+      <c r="C277" t="str">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278"/>
+      <c r="B278"/>
+      <c r="C278" t="str">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279"/>
+      <c r="B279"/>
+      <c r="C279" t="str">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280"/>
+      <c r="B280"/>
+      <c r="C280" t="str">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281"/>
+      <c r="B281"/>
+      <c r="C281" t="str">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282"/>
+      <c r="B282"/>
+      <c r="C282" t="str">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283"/>
+      <c r="B283"/>
+      <c r="C283" t="str">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284"/>
+      <c r="B284"/>
+      <c r="C284" t="str">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285"/>
+      <c r="B285"/>
+      <c r="C285" t="str">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286"/>
+      <c r="B286"/>
+      <c r="C286" t="str">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287"/>
+      <c r="B287"/>
+      <c r="C287" t="str">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288"/>
+      <c r="B288"/>
+      <c r="C288" t="str">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289"/>
+      <c r="B289"/>
+      <c r="C289" t="str">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290"/>
+      <c r="B290"/>
+      <c r="C290" t="str">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291"/>
+      <c r="B291"/>
+      <c r="C291" t="str">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292"/>
+      <c r="B292"/>
+      <c r="C292" t="str">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293"/>
+      <c r="B293"/>
+      <c r="C293" t="str">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294"/>
+      <c r="B294"/>
+      <c r="C294" t="str">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295"/>
+      <c r="B295"/>
+      <c r="C295" t="str">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296"/>
+      <c r="B296"/>
+      <c r="C296" t="str">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297"/>
+      <c r="B297"/>
+      <c r="C297" t="str">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298"/>
+      <c r="B298"/>
+      <c r="C298" t="str">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299"/>
+      <c r="B299"/>
+      <c r="C299" t="str">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300"/>
+      <c r="B300"/>
+      <c r="C300" t="str">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup scale="0" firstPageNumber="0" fitToWidth="0" fitToHeight="0" usePrinterDefaults="false" blackAndWhite="false" draft="false" useFirstPageNumber="false" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter differentFirst="false" differentOddEven="false"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr filterMode="false"/>
+  <dimension ref=""/>
+  <sheetViews/>
+  <sheetFormatPr defaultRowHeight="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup scale="0" firstPageNumber="0" fitToWidth="0" fitToHeight="0" usePrinterDefaults="false" blackAndWhite="false" draft="false" useFirstPageNumber="false" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter differentFirst="false" differentOddEven="false"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr filterMode="false"/>
+  <dimension ref=""/>
+  <sheetViews/>
+  <sheetFormatPr defaultRowHeight="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup scale="0" firstPageNumber="0" fitToWidth="0" fitToHeight="0" usePrinterDefaults="false" blackAndWhite="false" draft="false" useFirstPageNumber="false" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter differentFirst="false" differentOddEven="false"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix hyperlink missing after save issue and update completion row element logic to enhance compatibility.
</commit_message>
<xml_diff>
--- a/test/Workbook1.xlsx
+++ b/test/Workbook1.xlsx
@@ -2460,7 +2460,15 @@
         <v>0</v>
       </c>
     </row>
+    <row r="22" spans="2:2">
+      <c r="A22" t="str">
+        <v>GitHub</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A22" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
- Fix issue comments missing after save; - Update import PKG syntax in struct; - Update test XLSX file (include table, charts, functions, comments and hyperlink on Sheet1)
</commit_message>
<xml_diff>
--- a/test/Workbook1.xlsx
+++ b/test/Workbook1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27417"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xuri/Sites/repo/excelize/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xuri/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,8 +27,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="A22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Hyperlink test</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>IBM</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -78,12 +110,24 @@
   <si>
     <t>Other</t>
   </si>
+  <si>
+    <t>GitHub</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -104,6 +148,17 @@
       <name val="微软雅黑"/>
       <family val="2"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -778,11 +833,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="-493998416"/>
-        <c:axId val="-493993888"/>
+        <c:axId val="-217443504"/>
+        <c:axId val="-323855456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-493998416"/>
+        <c:axId val="-217443504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -825,7 +880,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-493993888"/>
+        <c:crossAx val="-323855456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -833,7 +888,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-493993888"/>
+        <c:axId val="-323855456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -883,7 +938,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-493998416"/>
+        <c:crossAx val="-217443504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2180,6 +2235,17 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C21:D26" totalsRowShown="0">
+  <autoFilter ref="C21:D26"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Column2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2443,35 +2509,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A19:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="19" spans="2:2">
-      <c r="A19" t="str">
-        <v>Total:</v>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>17</v>
       </c>
       <c r="B19">
         <f>SUM(Sheet2!D2,Sheet2!D11)</f>
-        <v>0</v>
+        <v>237</v>
       </c>
     </row>
-    <row r="22" spans="2:2">
-      <c r="A22" t="str">
-        <v>GitHub</v>
+    <row r="21" spans="1:4">
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A22" r:id="rId2"/>
+    <hyperlink ref="A22" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <picture r:id="rId3"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <picture r:id="rId4"/>
+  <tableParts count="1">
+    <tablePart r:id="rId5"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Support add picture with offset and scaling.
</commit_message>
<xml_diff>
--- a/test/Workbook1.xlsx
+++ b/test/Workbook1.xlsx
@@ -2516,6 +2516,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" width="5" max="6" min="6"/>
+  </cols>
   <sheetData>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
@@ -2534,7 +2537,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" customHeight="1" ht="25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -2562,6 +2565,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col customWidth="1" width="0.5" max="3" min="3"/>
+    <col customWidth="1" width="0" max="9" min="9"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2653,7 +2660,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2" customHeight="1" ht="0">
       <c r="C9" s="4" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
- Initialize shape support: new function `AddShape()` added. Relate issue #38; - Drawing `nvPicPr` element ID property calculation changed; - go test updated
</commit_message>
<xml_diff>
--- a/test/Workbook1.xlsx
+++ b/test/Workbook1.xlsx
@@ -751,27 +751,6 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -862,11 +841,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="-217443504"/>
-        <c:axId val="-323855456"/>
+        <c:axId val="754001152"/>
+        <c:axId val="753999904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-217443504"/>
+        <c:axId val="754001152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -909,7 +888,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-323855456"/>
+        <c:crossAx val="753999904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -917,7 +896,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-323855456"/>
+        <c:axId val="753999904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -967,7 +946,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-217443504"/>
+        <c:crossAx val="754001152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>

<commit_message>
Handle number formats out of built-in range exception by returning raw value, relate issue #50.
</commit_message>
<xml_diff>
--- a/test/Workbook1.xlsx
+++ b/test/Workbook1.xlsx
@@ -156,6 +156,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="177" formatCode="General"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -244,6 +247,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2631,7 +2637,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1">

</xml_diff>

<commit_message>
...move 'format' at own package
</commit_message>
<xml_diff>
--- a/test/Workbook1.xlsx
+++ b/test/Workbook1.xlsx
@@ -56,6 +56,9 @@
     <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rename Maximum 31 characters al" sheetId="50" relationships:id="rId50"/>
     <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rename Maximum 31 characters al" sheetId="51" relationships:id="rId51"/>
     <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rename Maximum 31 characters al" sheetId="52" relationships:id="rId52"/>
+    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rename Maximum 31 characters al" sheetId="53" relationships:id="rId53"/>
+    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rename Maximum 31 characters al" sheetId="54" relationships:id="rId54"/>
+    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rename Maximum 31 characters al" sheetId="55" relationships:id="rId55"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="false"/>
   <extLst>
@@ -2742,6 +2745,12 @@
     <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G10" relationships:id="rId98"/>
     <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B19" relationships:id="rId99"/>
     <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G10" relationships:id="rId100"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B19" relationships:id="rId101"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G10" relationships:id="rId102"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B19" relationships:id="rId103"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G10" relationships:id="rId104"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B19" relationships:id="rId105"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G10" relationships:id="rId106"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" relationships:id="rId2"/>
@@ -3149,7 +3158,7 @@
         <v>200</v>
       </c>
       <c r="G4" s="5">
-        <v>42962.7562181481</v>
+        <v>42962.825012985486</v>
       </c>
     </row>
     <row ht="17" r="5" spans="1:4">
@@ -3311,9 +3320,15 @@
     <hyperlink ref="D6" location="Sheet1!D8"/>
     <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C1" relationships:id="rId139"/>
     <hyperlink ref="D6" location="Sheet1!D8"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C1" relationships:id="rId142"/>
+    <hyperlink ref="D6" location="Sheet1!D8"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C1" relationships:id="rId145"/>
+    <hyperlink ref="D6" location="Sheet1!D8"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C1" relationships:id="rId148"/>
+    <hyperlink ref="D6" location="Sheet1!D8"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <picture xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" relationships:id="rId141"/>
+  <picture xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" relationships:id="rId150"/>
 </worksheet>
 </file>
 
@@ -5090,6 +5105,30 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <dimension ref=""/>
+  <sheetViews/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <dimension ref=""/>
+  <sheetViews/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <dimension ref=""/>
+  <sheetViews/>
+  <sheetData/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <dimension ref=""/>

</xml_diff>

<commit_message>
import 'format' package from 'xuri' repository
</commit_message>
<xml_diff>
--- a/test/Workbook1.xlsx
+++ b/test/Workbook1.xlsx
@@ -67,6 +67,7 @@
     <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rename Maximum 31 characters al" sheetId="61" relationships:id="rId61"/>
     <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rename Maximum 31 characters al" sheetId="62" relationships:id="rId62"/>
     <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rename Maximum 31 characters al" sheetId="63" relationships:id="rId63"/>
+    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rename Maximum 31 characters al" sheetId="64" relationships:id="rId64"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="false"/>
   <extLst>
@@ -2775,6 +2776,8 @@
     <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G10" relationships:id="rId120"/>
     <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B19" relationships:id="rId121"/>
     <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G10" relationships:id="rId122"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B19" relationships:id="rId123"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G10" relationships:id="rId124"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" relationships:id="rId2"/>
@@ -3182,7 +3185,7 @@
         <v>200</v>
       </c>
       <c r="G4" s="5">
-        <v>42962.89001914977</v>
+        <v>42962.89279706685</v>
       </c>
     </row>
     <row ht="17" r="5" spans="1:4">
@@ -3366,9 +3369,11 @@
     <hyperlink ref="D6" location="Sheet1!D8"/>
     <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C1" relationships:id="rId172"/>
     <hyperlink ref="D6" location="Sheet1!D8"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C1" relationships:id="rId175"/>
+    <hyperlink ref="D6" location="Sheet1!D8"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <picture xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" relationships:id="rId174"/>
+  <picture xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" relationships:id="rId177"/>
 </worksheet>
 </file>
 
@@ -5241,6 +5246,14 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <dimension ref=""/>
+  <sheetViews/>
+  <sheetData/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <dimension ref=""/>

</xml_diff>

<commit_message>
Add a test wich proves there is a issue with copySheet method
</commit_message>
<xml_diff>
--- a/test/Workbook1.xlsx
+++ b/test/Workbook1.xlsx
@@ -3,19 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xuri/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13220" yWindow="6260" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView activeTab="1" tabRatio="500" windowHeight="16880" windowWidth="28160" xWindow="13220" yWindow="6260"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" relationships:id="rId1"/>
+    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" relationships:id="rId2"/>
+    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rename Maximum 31 characters al" sheetId="6" relationships:id="rId6"/>
+    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rename Maximum 31 characters al" sheetId="7" relationships:id="rId7"/>
+    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rename Maximum 31 characters al" sheetId="8" relationships:id="rId8"/>
+    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rename Maximum 31 characters al" sheetId="9" relationships:id="rId9"/>
+    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rename Maximum 31 characters al" sheetId="10" relationships:id="rId10"/>
+    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rename Maximum 31 characters al" sheetId="11" relationships:id="rId11"/>
+    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rename Maximum 31 characters al" sheetId="12" relationships:id="rId12"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="false"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -155,11 +157,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="177" formatCode="General"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -193,12 +195,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill patternType="none">
+        <fgColor/>
+        <bgColor/>
+      </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor/>
+        <bgColor/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -206,8 +214,9 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill/>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -217,45 +226,55 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="2" tint="-9.9948118533890809E-2"/>
+        <color theme="2" tint="-0.09994811853389081"/>
       </left>
       <right style="thin">
-        <color theme="2" tint="-9.9948118533890809E-2"/>
+        <color theme="2" tint="-0.09994811853389081"/>
       </right>
       <top style="thin">
-        <color theme="2" tint="-9.9948118533890809E-2"/>
+        <color theme="2" tint="-0.09994811853389081"/>
       </top>
       <bottom style="thin">
-        <color theme="2" tint="-9.9948118533890809E-2"/>
+        <color theme="2" tint="-0.09994811853389081"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="6">
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="177" xfId="0">
       <alignment horizontal="left"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="2" fillId="3" fontId="0" numFmtId="22" xfId="0">
+      <alignment/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2521,27 +2540,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <dimension ref="A19:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView defaultGridColor="false" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" width="5" max="6" min="6"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="6" min="6" style="0" width="5"/>
   </cols>
   <sheetData>
+    <row r="1"/>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10">
+      <c r="G10">
+        <f>SUM(Sheet1!B19,Sheet1!C19)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19">
         <f>SUM(Sheet2!D2,Sheet2!D11)</f>
-        <v>237</v>
-      </c>
-    </row>
+      </c>
+      <c r="C19">
+        <f>SUM(Sheet2!D2,Sheet2!D9)</f>
+      </c>
+    </row>
+    <row r="20"/>
     <row r="21" spans="1:4">
       <c r="C21" t="s">
         <v>18</v>
@@ -2550,51 +2595,319 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4" customHeight="1" ht="25">
+    <row customHeight="true" ht="25" r="22" spans="1:4">
       <c r="A22" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells>
+    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="D11:F13"/>
+    <mergeCell ref="G10:K12"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A22" r:id="rId1"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A22" relationships:id="rId1"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B19" relationships:id="rId7"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G10" relationships:id="rId8"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B19" relationships:id="rId9"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G10" relationships:id="rId10"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B19" relationships:id="rId11"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G10" relationships:id="rId12"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B19" relationships:id="rId13"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G10" relationships:id="rId14"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B19" relationships:id="rId15"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G10" relationships:id="rId16"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B19" relationships:id="rId17"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G10" relationships:id="rId18"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B19" relationships:id="rId19"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="G10" relationships:id="rId20"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <picture r:id="rId4"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" relationships:id="rId2"/>
+  <legacyDrawing xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" relationships:id="rId3"/>
+  <picture xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" relationships:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" relationships:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <dimension ref=""/>
+  <sheetViews/>
+  <sheetData>
+    <row r="1"/>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65"/>
+    <row r="66"/>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70"/>
+    <row r="71"/>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81"/>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="87"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93"/>
+    <row r="94"/>
+    <row r="95"/>
+    <row r="96"/>
+    <row r="97"/>
+    <row r="98"/>
+    <row r="99"/>
+    <row r="100"/>
+    <row r="101"/>
+    <row r="102"/>
+    <row r="103"/>
+    <row r="104"/>
+    <row r="105"/>
+    <row r="106"/>
+    <row r="107"/>
+    <row r="108"/>
+    <row r="109"/>
+    <row r="110"/>
+    <row r="111"/>
+    <row r="112"/>
+    <row r="113"/>
+    <row r="114"/>
+    <row r="115"/>
+    <row r="116"/>
+    <row r="117"/>
+    <row r="118"/>
+    <row r="119"/>
+    <row r="120"/>
+    <row r="121"/>
+    <row r="122"/>
+    <row r="123"/>
+    <row r="124"/>
+    <row r="125"/>
+    <row r="126"/>
+    <row r="127"/>
+    <row r="128"/>
+    <row r="129"/>
+    <row r="130"/>
+    <row r="131"/>
+    <row r="132"/>
+    <row r="133"/>
+    <row r="134"/>
+    <row r="135"/>
+    <row r="136"/>
+    <row r="137"/>
+    <row r="138"/>
+    <row r="139"/>
+    <row r="140"/>
+    <row r="141"/>
+    <row r="142"/>
+    <row r="143"/>
+    <row r="144"/>
+    <row r="145"/>
+    <row r="146"/>
+    <row r="147"/>
+    <row r="148"/>
+    <row r="149"/>
+    <row r="150"/>
+    <row r="151"/>
+    <row r="152"/>
+    <row r="153"/>
+    <row r="154"/>
+    <row r="155"/>
+    <row r="156"/>
+    <row r="157"/>
+    <row r="158"/>
+    <row r="159"/>
+    <row r="160"/>
+    <row r="161"/>
+    <row r="162"/>
+    <row r="163"/>
+    <row r="164"/>
+    <row r="165"/>
+    <row r="166"/>
+    <row r="167"/>
+    <row r="168"/>
+    <row r="169"/>
+    <row r="170"/>
+    <row r="171"/>
+    <row r="172"/>
+    <row r="173"/>
+    <row r="174"/>
+    <row r="175"/>
+    <row r="176"/>
+    <row r="177"/>
+    <row r="178"/>
+    <row r="179"/>
+    <row r="180"/>
+    <row r="181"/>
+    <row r="182"/>
+    <row r="183"/>
+    <row r="184"/>
+    <row r="185"/>
+    <row r="186"/>
+    <row r="187"/>
+    <row r="188"/>
+    <row r="189"/>
+    <row r="190"/>
+    <row r="191"/>
+    <row r="192"/>
+    <row r="193"/>
+    <row r="194"/>
+    <row r="195"/>
+    <row r="196"/>
+    <row r="197"/>
+    <row r="198"/>
+    <row r="199"/>
+    <row r="200"/>
+    <row r="201"/>
+    <row r="202"/>
+    <row r="203"/>
+    <row r="204"/>
+    <row r="205"/>
+    <row r="206"/>
+    <row r="207"/>
+    <row r="208"/>
+    <row r="209"/>
+    <row r="210"/>
+    <row r="211"/>
+    <row r="212"/>
+    <row r="213"/>
+    <row r="214"/>
+    <row r="215"/>
+    <row r="216"/>
+    <row r="217"/>
+    <row r="218"/>
+    <row r="219"/>
+    <row r="220"/>
+    <row r="221"/>
+    <row r="222"/>
+    <row r="223"/>
+    <row r="224"/>
+    <row r="225"/>
+    <row r="226"/>
+    <row r="227"/>
+    <row r="228"/>
+    <row r="229"/>
+    <row r="230">
+      <c r="B230" t="str">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="true" defaultGridColor="false" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col customWidth="1" width="0.5" max="3" min="3"/>
-    <col max="7" min="7" style="0"/>
-    <col customWidth="1" width="0" max="9" min="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="3" min="3" style="0" width="0.5"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="9" min="9" style="0" width="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
+    <row ht="17" r="1" spans="1:4">
+      <c r="A1" s="1">
+        <v>100</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="F1" t="str" xml:space="preserve">
+        <v> Hello</v>
+      </c>
+      <c r="G1" t="str">
+        <v>World</v>
+      </c>
+    </row>
+    <row ht="17" r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -2607,8 +2920,13 @@
       <c r="D2" s="4">
         <v>200</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>42</v>
+      </c>
+      <c r="G2" t="str"/>
+      <c r="M2" t="str"/>
+    </row>
+    <row ht="17" r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2621,8 +2939,11 @@
       <c r="D3" s="4">
         <v>450</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="G3" t="str">
+        <v>8</v>
+      </c>
+    </row>
+    <row ht="17" r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -2635,8 +2956,11 @@
       <c r="D4" s="4">
         <v>200</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="G4" s="5">
+        <v>42964.82451761664</v>
+      </c>
+    </row>
+    <row ht="17" r="5" spans="1:4">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -2650,7 +2974,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
@@ -2658,7 +2982,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="C7" s="3" t="s">
         <v>0</v>
       </c>
@@ -2666,7 +2990,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
@@ -2674,7 +2998,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2" customHeight="1" ht="0">
+    <row customHeight="true" r="9" spans="1:4">
       <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
@@ -2682,7 +3006,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="C10" s="4" t="s">
         <v>10</v>
       </c>
@@ -2690,16 +3014,1598 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="C11" s="4" t="str">
-        <v>Other</v>
-      </c>
-      <c r="D11" s="4">
+        <v>Knowns</v>
+      </c>
+      <c r="D11" s="4" t="str">
+        <v>ccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccccc</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C1" relationships:id="rId1"/>
+    <hyperlink ref="D6" location="Sheet1!D8"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C1" relationships:id="rId4"/>
+    <hyperlink ref="D6" location="Sheet1!D8"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C1" relationships:id="rId7"/>
+    <hyperlink ref="D6" location="Sheet1!D8"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C1" relationships:id="rId10"/>
+    <hyperlink ref="D6" location="Sheet1!D8"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C1" relationships:id="rId13"/>
+    <hyperlink ref="D6" location="Sheet1!D8"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C1" relationships:id="rId16"/>
+    <hyperlink ref="D6" location="Sheet1!D8"/>
+    <hyperlink xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C1" relationships:id="rId19"/>
+    <hyperlink ref="D6" location="Sheet1!D8"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <picture xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" relationships:id="rId21"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView defaultGridColor="false" workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="C1" t="str">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" t="str">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" t="str">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" t="str">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="str">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="str">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" t="str">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" t="str">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" t="str">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" t="str">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" t="str">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" t="str">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" t="str">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" t="str">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" t="str">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" t="str">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" t="str">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" t="str">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" t="str">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" t="str">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" t="str">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>10</v>
+      </c>
+      <c r="C23" t="str">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="C24" t="str">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" t="str">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="C26" t="str">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="C27" t="str">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="C28" t="str">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" t="str">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="C30" t="str">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="C31" t="str">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="C32" t="str">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="C33" t="str">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="C34" t="str">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="C35" t="str">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="C36" t="str">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="C37" t="str">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2"/>
+    <row r="38">
+      <c r="C38" t="str">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="C39" t="str">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="C40" t="str">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="C41" t="str">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="C42" t="str">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="C43" t="str">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="C44" t="str">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="C45" t="str">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="C46" t="str">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="C47" t="str">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="C48" t="str">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="C49" t="str">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="C50" t="str">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="C51" t="str">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="C52" t="str">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="C53" t="str">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="C54" t="str">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="C55" t="str">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="C56" t="str">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="C57" t="str">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="C58" t="str">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="C59" t="str">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="C60" t="str">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="C61" t="str">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="C62" t="str">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="C63" t="str">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="C64" t="str">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="C65" t="str">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="C66" t="str">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="C67" t="str">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="C68" t="str">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="C69" t="str">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="C70" t="str">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="C71" t="str">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="C72" t="str">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="C73" t="str">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="C74" t="str">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="C75" t="str">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="C76" t="str">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="C77" t="str">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="C78" t="str">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="C79" t="str">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="C80" t="str">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="C81" t="str">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="C82" t="str">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="C83" t="str">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="C84" t="str">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="C85" t="str">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="C86" t="str">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="C87" t="str">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="C88" t="str">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="C89" t="str">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="C90" t="str">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="C91" t="str">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="C92" t="str">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="C93" t="str">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="C94" t="str">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="C95" t="str">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="C96" t="str">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="C97" t="str">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="C98" t="str">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="C99" t="str">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="C100" t="str">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="C101" t="str">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="C102" t="str">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="C103" t="str">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="C104" t="str">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="C105" t="str">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="C106" t="str">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="C107" t="str">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="C108" t="str">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="C109" t="str">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="C110" t="str">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="C111" t="str">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="C112" t="str">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="C113" t="str">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="C114" t="str">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="C115" t="str">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="C116" t="str">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="C117" t="str">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="C118" t="str">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="C119" t="str">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="C120" t="str">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="C121" t="str">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="C122" t="str">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="C123" t="str">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="C124" t="str">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="C125" t="str">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="C126" t="str">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="C127" t="str">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="C128" t="str">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="C129" t="str">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="C130" t="str">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="C131" t="str">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="C132" t="str">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="C133" t="str">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="C134" t="str">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="C135" t="str">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="C136" t="str">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="C137" t="str">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="C138" t="str">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="C139" t="str">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="C140" t="str">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="C141" t="str">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="C142" t="str">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="C143" t="str">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="C144" t="str">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="C145" t="str">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="C146" t="str">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="C147" t="str">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="C148" t="str">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="C149" t="str">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="C150" t="str">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="C151" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="C152" t="str">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="C153" t="str">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="C154" t="str">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="C155" t="str">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="C156" t="str">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="C157" t="str">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="C158" t="str">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="C159" t="str">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="C160" t="str">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="C161" t="str">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="C162" t="str">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="C163" t="str">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="C164" t="str">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="C165" t="str">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="C166" t="str">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="C167" t="str">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="C168" t="str">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="C169" t="str">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="C170" t="str">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="C171" t="str">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="C172" t="str">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="C173" t="str">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="C174" t="str">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="C175" t="str">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="C176" t="str">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="C177" t="str">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="C178" t="str">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="C179" t="str">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="C180" t="str">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="C181" t="str">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="C182" t="str">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="C183" t="str">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="C184" t="str">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="C185" t="str">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="C186" t="str">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="C187" t="str">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="C188" t="str">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="C189" t="str">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="C190" t="str">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="C191" t="str">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="C192" t="str">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="C193" t="str">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="C194" t="str">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="C195" t="str">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="C196" t="str">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="C197" t="str">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="C198" t="str">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="C199" t="str">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="C200" t="str">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="C201" t="str">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="C202" t="str">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="C203" t="str">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="C204" t="str">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="C205" t="str">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="C206" t="str">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="C207" t="str">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="C208" t="str">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="C209" t="str">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="C210" t="str">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="C211" t="str">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="C212" t="str">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="C213" t="str">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="C214" t="str">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="C215" t="str">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="C216" t="str">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="C217" t="str">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="C218" t="str">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="C219" t="str">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="C220" t="str">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="C221" t="str">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="C222" t="str">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="C223" t="str">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="C224" t="str">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="C225" t="str">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="C226" t="str">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="C227" t="str">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="C228" t="str">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="C229" t="str">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="B230" t="str">
+        <v>10</v>
+      </c>
+      <c r="C230" t="str">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="C231" t="str">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="C232" t="str">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="C233" t="str">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="C234" t="str">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="C235" t="str">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="C236" t="str">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="C237" t="str">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="C238" t="str">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="C239" t="str">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="C240" t="str">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="C241" t="str">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="C242" t="str">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="C243" t="str">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="C244" t="str">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="C245" t="str">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="C246" t="str">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="C247" t="str">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="C248" t="str">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="C249" t="str">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="C250" t="str">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="C251" t="str">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="C252" t="str">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="C253" t="str">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="C254" t="str">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="C255" t="str">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="C256" t="str">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="C257" t="str">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="C258" t="str">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="C259" t="str">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="C260" t="str">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="C261" t="str">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="C262" t="str">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="C263" t="str">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="C264" t="str">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="C265" t="str">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="C266" t="str">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="C267" t="str">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="C268" t="str">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="C269" t="str">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="C270" t="str">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="C271" t="str">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="C272" t="str">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="C273" t="str">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="C274" t="str">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="C275" t="str">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="C276" t="str">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="C277" t="str">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="C278" t="str">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="C279" t="str">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="C280" t="str">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="C281" t="str">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="C282" t="str">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="C283" t="str">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="C284" t="str">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="C285" t="str">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="C286" t="str">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="C287" t="str">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="C288" t="str">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="C289" t="str">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="C290" t="str">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="C291" t="str">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="C292" t="str">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="C293" t="str">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="C294" t="str">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="C295" t="str">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="C296" t="str">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="C297" t="str">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="C298" t="str">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="C299" t="str">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="C300" t="str">
+        <v>300</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <dimension ref=""/>
+  <sheetViews/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <dimension ref=""/>
+  <sheetViews/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <dimension ref=""/>
+  <sheetViews/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <dimension ref=""/>
+  <sheetViews/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <dimension ref=""/>
+  <sheetViews/>
+  <sheetData/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <dimension ref=""/>
+  <sheetViews/>
+  <sheetData/>
 </worksheet>
 </file>
</xml_diff>